<commit_message>
Prueba de visualización de rutas
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{99729213-C3B5-4607-9D2A-277AC7829DBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{315CCC2F-3160-4C47-9B34-19BD98A676CC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Flota Consolidado" sheetId="10" r:id="rId1"/>
@@ -269,7 +269,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4051" uniqueCount="625">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4057" uniqueCount="625">
   <si>
     <t>Región</t>
   </si>
@@ -4127,14 +4127,23 @@
       <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="40" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="40" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="39" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="33" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="55" fillId="28" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="24" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="35" fillId="4" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -4165,39 +4174,6 @@
     </xf>
     <xf numFmtId="0" fontId="37" fillId="23" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="39" fillId="9" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="40" fillId="19" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="26" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="25" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="22" borderId="15" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -4266,6 +4242,30 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="25" fillId="21" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="26" fillId="19" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="18" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="19" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="20" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="9" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="10" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -23571,142 +23571,142 @@
   </cols>
   <sheetData>
     <row r="2" spans="1:39" ht="32.4">
-      <c r="A2" s="299" t="s">
+      <c r="A2" s="303" t="s">
         <v>250</v>
       </c>
-      <c r="B2" s="299"/>
-      <c r="C2" s="299"/>
+      <c r="B2" s="303"/>
+      <c r="C2" s="303"/>
     </row>
     <row r="4" spans="1:39" ht="4.8" customHeight="1">
       <c r="A4" s="170"/>
     </row>
     <row r="5" spans="1:39" ht="67.2" customHeight="1">
-      <c r="A5" s="302"/>
-      <c r="B5" s="302"/>
-      <c r="C5" s="302"/>
-      <c r="D5" s="303" t="s">
+      <c r="A5" s="305"/>
+      <c r="B5" s="305"/>
+      <c r="C5" s="305"/>
+      <c r="D5" s="306" t="s">
         <v>251</v>
       </c>
-      <c r="E5" s="303"/>
-      <c r="F5" s="303"/>
-      <c r="G5" s="303"/>
-      <c r="H5" s="303"/>
-      <c r="I5" s="304" t="s">
+      <c r="E5" s="306"/>
+      <c r="F5" s="306"/>
+      <c r="G5" s="306"/>
+      <c r="H5" s="306"/>
+      <c r="I5" s="307" t="s">
         <v>252</v>
       </c>
-      <c r="J5" s="304"/>
-      <c r="K5" s="304"/>
-      <c r="L5" s="304"/>
-      <c r="M5" s="305" t="s">
+      <c r="J5" s="307"/>
+      <c r="K5" s="307"/>
+      <c r="L5" s="307"/>
+      <c r="M5" s="308" t="s">
         <v>253</v>
       </c>
-      <c r="N5" s="305"/>
-      <c r="O5" s="307" t="s">
+      <c r="N5" s="308"/>
+      <c r="O5" s="310" t="s">
         <v>254</v>
       </c>
-      <c r="P5" s="307"/>
-      <c r="Q5" s="308" t="s">
+      <c r="P5" s="310"/>
+      <c r="Q5" s="311" t="s">
         <v>255</v>
       </c>
-      <c r="R5" s="308"/>
-      <c r="S5" s="309" t="s">
+      <c r="R5" s="311"/>
+      <c r="S5" s="312" t="s">
         <v>256</v>
       </c>
-      <c r="T5" s="309"/>
-      <c r="U5" s="309"/>
-      <c r="V5" s="309"/>
-      <c r="W5" s="309"/>
-      <c r="X5" s="309"/>
-      <c r="Y5" s="309"/>
-      <c r="Z5" s="309"/>
-      <c r="AA5" s="309"/>
-      <c r="AB5" s="309"/>
-      <c r="AC5" s="310" t="s">
+      <c r="T5" s="312"/>
+      <c r="U5" s="312"/>
+      <c r="V5" s="312"/>
+      <c r="W5" s="312"/>
+      <c r="X5" s="312"/>
+      <c r="Y5" s="312"/>
+      <c r="Z5" s="312"/>
+      <c r="AA5" s="312"/>
+      <c r="AB5" s="312"/>
+      <c r="AC5" s="313" t="s">
         <v>257</v>
       </c>
-      <c r="AD5" s="310"/>
-      <c r="AE5" s="310"/>
-      <c r="AF5" s="310"/>
-      <c r="AG5" s="311" t="s">
+      <c r="AD5" s="313"/>
+      <c r="AE5" s="313"/>
+      <c r="AF5" s="313"/>
+      <c r="AG5" s="314" t="s">
         <v>258</v>
       </c>
-      <c r="AH5" s="311"/>
-      <c r="AI5" s="311"/>
-      <c r="AJ5" s="311"/>
-      <c r="AK5" s="311"/>
-      <c r="AL5" s="311"/>
-      <c r="AM5" s="311"/>
+      <c r="AH5" s="314"/>
+      <c r="AI5" s="314"/>
+      <c r="AJ5" s="314"/>
+      <c r="AK5" s="314"/>
+      <c r="AL5" s="314"/>
+      <c r="AM5" s="314"/>
     </row>
     <row r="6" spans="1:39" ht="21.6">
-      <c r="A6" s="302"/>
-      <c r="B6" s="302"/>
-      <c r="C6" s="302"/>
-      <c r="D6" s="303"/>
-      <c r="E6" s="303"/>
-      <c r="F6" s="303"/>
-      <c r="G6" s="303"/>
-      <c r="H6" s="303"/>
-      <c r="I6" s="304"/>
-      <c r="J6" s="304"/>
-      <c r="K6" s="304"/>
-      <c r="L6" s="304"/>
-      <c r="M6" s="305"/>
-      <c r="N6" s="305"/>
-      <c r="O6" s="307"/>
-      <c r="P6" s="307"/>
-      <c r="Q6" s="308"/>
-      <c r="R6" s="308"/>
-      <c r="S6" s="312" t="s">
+      <c r="A6" s="305"/>
+      <c r="B6" s="305"/>
+      <c r="C6" s="305"/>
+      <c r="D6" s="306"/>
+      <c r="E6" s="306"/>
+      <c r="F6" s="306"/>
+      <c r="G6" s="306"/>
+      <c r="H6" s="306"/>
+      <c r="I6" s="307"/>
+      <c r="J6" s="307"/>
+      <c r="K6" s="307"/>
+      <c r="L6" s="307"/>
+      <c r="M6" s="308"/>
+      <c r="N6" s="308"/>
+      <c r="O6" s="310"/>
+      <c r="P6" s="310"/>
+      <c r="Q6" s="311"/>
+      <c r="R6" s="311"/>
+      <c r="S6" s="301" t="s">
         <v>259</v>
       </c>
-      <c r="T6" s="312"/>
-      <c r="U6" s="312" t="s">
+      <c r="T6" s="301"/>
+      <c r="U6" s="301" t="s">
         <v>260</v>
       </c>
-      <c r="V6" s="312"/>
-      <c r="W6" s="313" t="s">
+      <c r="V6" s="301"/>
+      <c r="W6" s="302" t="s">
         <v>261</v>
       </c>
-      <c r="X6" s="313"/>
-      <c r="Y6" s="312" t="s">
+      <c r="X6" s="302"/>
+      <c r="Y6" s="301" t="s">
         <v>262</v>
       </c>
-      <c r="Z6" s="312"/>
-      <c r="AA6" s="312" t="s">
+      <c r="Z6" s="301"/>
+      <c r="AA6" s="301" t="s">
         <v>263</v>
       </c>
-      <c r="AB6" s="312"/>
-      <c r="AC6" s="314" t="s">
+      <c r="AB6" s="301"/>
+      <c r="AC6" s="300" t="s">
         <v>264</v>
       </c>
-      <c r="AD6" s="314" t="s">
+      <c r="AD6" s="300" t="s">
         <v>265</v>
       </c>
-      <c r="AE6" s="314" t="s">
+      <c r="AE6" s="300" t="s">
         <v>266</v>
       </c>
-      <c r="AF6" s="314" t="s">
+      <c r="AF6" s="300" t="s">
         <v>267</v>
       </c>
-      <c r="AG6" s="301" t="s">
+      <c r="AG6" s="299" t="s">
         <v>268</v>
       </c>
-      <c r="AH6" s="301" t="s">
+      <c r="AH6" s="299" t="s">
         <v>269</v>
       </c>
-      <c r="AI6" s="301" t="s">
+      <c r="AI6" s="299" t="s">
         <v>270</v>
       </c>
-      <c r="AJ6" s="301" t="s">
+      <c r="AJ6" s="299" t="s">
         <v>271</v>
       </c>
-      <c r="AK6" s="301" t="s">
+      <c r="AK6" s="299" t="s">
         <v>272</v>
       </c>
-      <c r="AL6" s="301" t="s">
+      <c r="AL6" s="299" t="s">
         <v>273</v>
       </c>
-      <c r="AM6" s="301" t="s">
+      <c r="AM6" s="299" t="s">
         <v>274</v>
       </c>
     </row>
@@ -23795,17 +23795,17 @@
       <c r="AB7" s="179" t="s">
         <v>292</v>
       </c>
-      <c r="AC7" s="314"/>
-      <c r="AD7" s="314"/>
-      <c r="AE7" s="314"/>
-      <c r="AF7" s="314"/>
-      <c r="AG7" s="301"/>
-      <c r="AH7" s="301"/>
-      <c r="AI7" s="301"/>
-      <c r="AJ7" s="301"/>
-      <c r="AK7" s="301"/>
-      <c r="AL7" s="301"/>
-      <c r="AM7" s="301"/>
+      <c r="AC7" s="300"/>
+      <c r="AD7" s="300"/>
+      <c r="AE7" s="300"/>
+      <c r="AF7" s="300"/>
+      <c r="AG7" s="299"/>
+      <c r="AH7" s="299"/>
+      <c r="AI7" s="299"/>
+      <c r="AJ7" s="299"/>
+      <c r="AK7" s="299"/>
+      <c r="AL7" s="299"/>
+      <c r="AM7" s="299"/>
     </row>
     <row r="8" spans="1:39" s="212" customFormat="1" ht="23.4">
       <c r="A8" s="202">
@@ -28679,11 +28679,11 @@
     </row>
     <row r="49" spans="1:39" ht="21">
       <c r="A49" s="217"/>
-      <c r="B49" s="306" t="s">
+      <c r="B49" s="309" t="s">
         <v>391</v>
       </c>
-      <c r="C49" s="306"/>
-      <c r="D49" s="306"/>
+      <c r="C49" s="309"/>
+      <c r="D49" s="309"/>
       <c r="E49" s="218"/>
       <c r="F49" s="218"/>
       <c r="G49" s="218"/>
@@ -29435,11 +29435,11 @@
       </c>
     </row>
     <row r="58" spans="1:39" ht="21">
-      <c r="A58" s="300" t="s">
+      <c r="A58" s="304" t="s">
         <v>406</v>
       </c>
-      <c r="B58" s="300"/>
-      <c r="C58" s="300"/>
+      <c r="B58" s="304"/>
+      <c r="C58" s="304"/>
     </row>
     <row r="59" spans="1:39" s="212" customFormat="1" ht="23.4">
       <c r="A59" s="202">
@@ -31220,18 +31220,6 @@
     </row>
   </sheetData>
   <mergeCells count="28">
-    <mergeCell ref="AL6:AL7"/>
-    <mergeCell ref="AM6:AM7"/>
-    <mergeCell ref="AD6:AD7"/>
-    <mergeCell ref="AE6:AE7"/>
-    <mergeCell ref="AF6:AF7"/>
-    <mergeCell ref="AG6:AG7"/>
-    <mergeCell ref="AH6:AH7"/>
-    <mergeCell ref="U6:V6"/>
-    <mergeCell ref="W6:X6"/>
-    <mergeCell ref="Y6:Z6"/>
-    <mergeCell ref="AA6:AB6"/>
-    <mergeCell ref="AC6:AC7"/>
     <mergeCell ref="A2:C2"/>
     <mergeCell ref="A58:C58"/>
     <mergeCell ref="AI6:AI7"/>
@@ -31248,6 +31236,18 @@
     <mergeCell ref="AC5:AF5"/>
     <mergeCell ref="AG5:AM5"/>
     <mergeCell ref="S6:T6"/>
+    <mergeCell ref="U6:V6"/>
+    <mergeCell ref="W6:X6"/>
+    <mergeCell ref="Y6:Z6"/>
+    <mergeCell ref="AA6:AB6"/>
+    <mergeCell ref="AC6:AC7"/>
+    <mergeCell ref="AL6:AL7"/>
+    <mergeCell ref="AM6:AM7"/>
+    <mergeCell ref="AD6:AD7"/>
+    <mergeCell ref="AE6:AE7"/>
+    <mergeCell ref="AF6:AF7"/>
+    <mergeCell ref="AG6:AG7"/>
+    <mergeCell ref="AH6:AH7"/>
   </mergeCells>
   <conditionalFormatting sqref="R7">
     <cfRule type="cellIs" dxfId="536" priority="316" operator="between">
@@ -32557,8 +32557,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:BM11"/>
   <sheetViews>
-    <sheetView topLeftCell="M1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S1" sqref="S1:AA1"/>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4"/>
@@ -32836,11 +32836,11 @@
       <c r="G2" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H2" s="39">
-        <v>1</v>
+      <c r="H2" s="39" t="s">
+        <v>613</v>
       </c>
       <c r="I2" s="39" t="s">
-        <v>613</v>
+        <v>59</v>
       </c>
       <c r="J2" s="40" t="s">
         <v>14</v>
@@ -32985,11 +32985,11 @@
       <c r="G3" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H3" s="39">
-        <v>2</v>
+      <c r="H3" s="39" t="s">
+        <v>614</v>
       </c>
       <c r="I3" s="39" t="s">
-        <v>614</v>
+        <v>59</v>
       </c>
       <c r="J3" s="40" t="s">
         <v>14</v>
@@ -33134,11 +33134,11 @@
       <c r="G4" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H4" s="39">
-        <v>3</v>
+      <c r="H4" s="39" t="s">
+        <v>615</v>
       </c>
       <c r="I4" s="39" t="s">
-        <v>615</v>
+        <v>59</v>
       </c>
       <c r="J4" s="40" t="s">
         <v>14</v>
@@ -33283,11 +33283,11 @@
       <c r="G5" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H5" s="39">
-        <v>4</v>
+      <c r="H5" s="39" t="s">
+        <v>616</v>
       </c>
       <c r="I5" s="39" t="s">
-        <v>616</v>
+        <v>59</v>
       </c>
       <c r="J5" s="40" t="s">
         <v>14</v>
@@ -33432,11 +33432,11 @@
       <c r="G6" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H6" s="39">
-        <v>5</v>
+      <c r="H6" s="39" t="s">
+        <v>612</v>
       </c>
       <c r="I6" s="39" t="s">
-        <v>612</v>
+        <v>59</v>
       </c>
       <c r="J6" s="40" t="s">
         <v>14</v>
@@ -33579,11 +33579,11 @@
       <c r="G7" s="37" t="s">
         <v>29</v>
       </c>
-      <c r="H7" s="39">
-        <v>6</v>
+      <c r="H7" s="39" t="s">
+        <v>617</v>
       </c>
       <c r="I7" s="39" t="s">
-        <v>617</v>
+        <v>59</v>
       </c>
       <c r="J7" s="40" t="s">
         <v>14</v>
@@ -34390,108 +34390,108 @@
       <c r="A1" s="72"/>
     </row>
     <row r="2" spans="1:40" ht="15">
-      <c r="A2" s="325"/>
-      <c r="B2" s="325"/>
-      <c r="C2" s="325"/>
-      <c r="D2" s="326" t="s">
+      <c r="A2" s="317"/>
+      <c r="B2" s="317"/>
+      <c r="C2" s="317"/>
+      <c r="D2" s="318" t="s">
         <v>251</v>
       </c>
-      <c r="E2" s="327"/>
-      <c r="F2" s="327"/>
-      <c r="G2" s="327"/>
-      <c r="H2" s="328"/>
-      <c r="I2" s="332" t="s">
+      <c r="E2" s="319"/>
+      <c r="F2" s="319"/>
+      <c r="G2" s="319"/>
+      <c r="H2" s="320"/>
+      <c r="I2" s="324" t="s">
         <v>252</v>
       </c>
-      <c r="J2" s="333"/>
-      <c r="K2" s="333"/>
-      <c r="L2" s="334"/>
-      <c r="M2" s="338" t="s">
+      <c r="J2" s="325"/>
+      <c r="K2" s="325"/>
+      <c r="L2" s="326"/>
+      <c r="M2" s="330" t="s">
         <v>253</v>
       </c>
-      <c r="N2" s="339"/>
-      <c r="O2" s="342" t="s">
+      <c r="N2" s="331"/>
+      <c r="O2" s="334" t="s">
         <v>254</v>
       </c>
-      <c r="P2" s="343"/>
-      <c r="Q2" s="323" t="s">
+      <c r="P2" s="335"/>
+      <c r="Q2" s="315" t="s">
         <v>255</v>
       </c>
-      <c r="R2" s="323"/>
-      <c r="S2" s="317" t="s">
+      <c r="R2" s="315"/>
+      <c r="S2" s="340" t="s">
         <v>256</v>
       </c>
-      <c r="T2" s="317"/>
-      <c r="U2" s="317"/>
-      <c r="V2" s="317"/>
-      <c r="W2" s="317"/>
-      <c r="X2" s="317"/>
-      <c r="Y2" s="317"/>
-      <c r="Z2" s="317"/>
-      <c r="AA2" s="317"/>
-      <c r="AB2" s="317"/>
-      <c r="AC2" s="317"/>
-      <c r="AD2" s="317"/>
-      <c r="AE2" s="318" t="s">
+      <c r="T2" s="340"/>
+      <c r="U2" s="340"/>
+      <c r="V2" s="340"/>
+      <c r="W2" s="340"/>
+      <c r="X2" s="340"/>
+      <c r="Y2" s="340"/>
+      <c r="Z2" s="340"/>
+      <c r="AA2" s="340"/>
+      <c r="AB2" s="340"/>
+      <c r="AC2" s="340"/>
+      <c r="AD2" s="340"/>
+      <c r="AE2" s="341" t="s">
         <v>433</v>
       </c>
-      <c r="AF2" s="318"/>
-      <c r="AG2" s="318"/>
-      <c r="AH2" s="318"/>
+      <c r="AF2" s="341"/>
+      <c r="AG2" s="341"/>
+      <c r="AH2" s="341"/>
     </row>
     <row r="3" spans="1:40" ht="15">
-      <c r="A3" s="325"/>
-      <c r="B3" s="325"/>
-      <c r="C3" s="325"/>
-      <c r="D3" s="329"/>
-      <c r="E3" s="330"/>
-      <c r="F3" s="330"/>
-      <c r="G3" s="330"/>
-      <c r="H3" s="331"/>
-      <c r="I3" s="335"/>
-      <c r="J3" s="336"/>
-      <c r="K3" s="336"/>
-      <c r="L3" s="337"/>
-      <c r="M3" s="340"/>
-      <c r="N3" s="341"/>
-      <c r="O3" s="344"/>
-      <c r="P3" s="345"/>
-      <c r="Q3" s="324"/>
-      <c r="R3" s="324"/>
-      <c r="S3" s="319" t="s">
+      <c r="A3" s="317"/>
+      <c r="B3" s="317"/>
+      <c r="C3" s="317"/>
+      <c r="D3" s="321"/>
+      <c r="E3" s="322"/>
+      <c r="F3" s="322"/>
+      <c r="G3" s="322"/>
+      <c r="H3" s="323"/>
+      <c r="I3" s="327"/>
+      <c r="J3" s="328"/>
+      <c r="K3" s="328"/>
+      <c r="L3" s="329"/>
+      <c r="M3" s="332"/>
+      <c r="N3" s="333"/>
+      <c r="O3" s="336"/>
+      <c r="P3" s="337"/>
+      <c r="Q3" s="316"/>
+      <c r="R3" s="316"/>
+      <c r="S3" s="342" t="s">
         <v>259</v>
       </c>
-      <c r="T3" s="320"/>
-      <c r="U3" s="319" t="s">
+      <c r="T3" s="343"/>
+      <c r="U3" s="342" t="s">
         <v>260</v>
       </c>
-      <c r="V3" s="320"/>
-      <c r="W3" s="319" t="s">
+      <c r="V3" s="343"/>
+      <c r="W3" s="342" t="s">
         <v>434</v>
       </c>
-      <c r="X3" s="320"/>
-      <c r="Y3" s="321" t="s">
+      <c r="X3" s="343"/>
+      <c r="Y3" s="344" t="s">
         <v>261</v>
       </c>
-      <c r="Z3" s="321"/>
-      <c r="AA3" s="322" t="s">
+      <c r="Z3" s="344"/>
+      <c r="AA3" s="345" t="s">
         <v>262</v>
       </c>
-      <c r="AB3" s="320"/>
-      <c r="AC3" s="322" t="s">
+      <c r="AB3" s="343"/>
+      <c r="AC3" s="345" t="s">
         <v>435</v>
       </c>
-      <c r="AD3" s="320"/>
-      <c r="AE3" s="315" t="s">
+      <c r="AD3" s="343"/>
+      <c r="AE3" s="338" t="s">
         <v>436</v>
       </c>
-      <c r="AF3" s="315" t="s">
+      <c r="AF3" s="338" t="s">
         <v>437</v>
       </c>
-      <c r="AG3" s="315" t="s">
+      <c r="AG3" s="338" t="s">
         <v>438</v>
       </c>
-      <c r="AH3" s="315" t="s">
+      <c r="AH3" s="338" t="s">
         <v>439</v>
       </c>
     </row>
@@ -34586,10 +34586,10 @@
       <c r="AD4" s="82" t="s">
         <v>292</v>
       </c>
-      <c r="AE4" s="316"/>
-      <c r="AF4" s="316"/>
-      <c r="AG4" s="316"/>
-      <c r="AH4" s="316"/>
+      <c r="AE4" s="339"/>
+      <c r="AF4" s="339"/>
+      <c r="AG4" s="339"/>
+      <c r="AH4" s="339"/>
       <c r="AI4" s="74" t="s">
         <v>270</v>
       </c>
@@ -36189,12 +36189,6 @@
     </row>
   </sheetData>
   <mergeCells count="18">
-    <mergeCell ref="Q2:R3"/>
-    <mergeCell ref="A2:C3"/>
-    <mergeCell ref="D2:H3"/>
-    <mergeCell ref="I2:L3"/>
-    <mergeCell ref="M2:N3"/>
-    <mergeCell ref="O2:P3"/>
     <mergeCell ref="AG3:AG4"/>
     <mergeCell ref="AH3:AH4"/>
     <mergeCell ref="S2:AD2"/>
@@ -36207,6 +36201,12 @@
     <mergeCell ref="AC3:AD3"/>
     <mergeCell ref="AE3:AE4"/>
     <mergeCell ref="AF3:AF4"/>
+    <mergeCell ref="Q2:R3"/>
+    <mergeCell ref="A2:C3"/>
+    <mergeCell ref="D2:H3"/>
+    <mergeCell ref="I2:L3"/>
+    <mergeCell ref="M2:N3"/>
+    <mergeCell ref="O2:P3"/>
   </mergeCells>
   <conditionalFormatting sqref="R4">
     <cfRule type="cellIs" dxfId="138" priority="138" operator="between">
@@ -36809,7 +36809,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0500-000000000000}">
   <dimension ref="A1:AP7"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
+    <sheetView topLeftCell="C1" workbookViewId="0">
       <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
Se une el JSON de unidades unificado con el resto del programa
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D4BBB52E-639B-481F-8445-F5F1D31B8253}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3115BF05-CC9A-473E-9631-2B4F451A8347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -694,7 +694,7 @@
   <dimension ref="A1:Q47"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q13" sqref="Q13"/>
+      <selection activeCell="T3" sqref="T3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -2705,5 +2705,6 @@
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se agrega nuevo campo de unidades disponibles
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3115BF05-CC9A-473E-9631-2B4F451A8347}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C80A4C-181C-4E3E-8880-D837BE074D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="246" uniqueCount="103">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
   <si>
     <t>Placa de tracto</t>
   </si>
@@ -329,13 +329,22 @@
   </si>
   <si>
     <t>AEO-992</t>
+  </si>
+  <si>
+    <t>Disponible</t>
+  </si>
+  <si>
+    <t>SI</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> </t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -347,6 +356,14 @@
       <b/>
       <sz val="11"/>
       <name val="Calibri"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -384,11 +401,12 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -691,10 +709,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:Q47"/>
+  <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T3" sqref="T3"/>
+    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
+      <selection activeCell="T43" sqref="T43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -708,9 +726,10 @@
     <col min="7" max="7" width="9.77734375" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="9" max="17" width="5" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="9.77734375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:17" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:18" x14ac:dyDescent="0.3">
       <c r="B1" s="1" t="s">
         <v>0</v>
       </c>
@@ -759,8 +778,11 @@
       <c r="Q1" s="1" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="2" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R1" s="1" t="s">
+        <v>103</v>
+      </c>
+    </row>
+    <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
         <v>0</v>
       </c>
@@ -800,8 +822,11 @@
       <c r="M2">
         <v>500</v>
       </c>
-    </row>
-    <row r="3" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R2" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -850,8 +875,11 @@
       <c r="P3">
         <v>1000</v>
       </c>
-    </row>
-    <row r="4" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R3" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
         <v>2</v>
       </c>
@@ -885,8 +913,11 @@
       <c r="K4">
         <v>2000</v>
       </c>
-    </row>
-    <row r="5" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R4" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
         <v>3</v>
       </c>
@@ -914,8 +945,11 @@
       <c r="I5">
         <v>9000</v>
       </c>
-    </row>
-    <row r="6" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R5" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
         <v>4</v>
       </c>
@@ -958,8 +992,11 @@
       <c r="N6">
         <v>500</v>
       </c>
-    </row>
-    <row r="7" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R6" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
         <v>5</v>
       </c>
@@ -1005,8 +1042,11 @@
       <c r="O7">
         <v>1000</v>
       </c>
-    </row>
-    <row r="8" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R7" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
         <v>6</v>
       </c>
@@ -1052,8 +1092,11 @@
       <c r="O8">
         <v>1000</v>
       </c>
-    </row>
-    <row r="9" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R8" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
         <v>7</v>
       </c>
@@ -1090,8 +1133,11 @@
       <c r="L9">
         <v>1500</v>
       </c>
-    </row>
-    <row r="10" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R9" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
         <v>8</v>
       </c>
@@ -1128,8 +1174,11 @@
       <c r="L10">
         <v>1000</v>
       </c>
-    </row>
-    <row r="11" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R10" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
         <v>9</v>
       </c>
@@ -1163,8 +1212,11 @@
       <c r="K11">
         <v>3000</v>
       </c>
-    </row>
-    <row r="12" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R11" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
         <v>10</v>
       </c>
@@ -1201,8 +1253,11 @@
       <c r="L12">
         <v>500</v>
       </c>
-    </row>
-    <row r="13" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R12" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
         <v>11</v>
       </c>
@@ -1239,8 +1294,11 @@
       <c r="L13">
         <v>1500</v>
       </c>
-    </row>
-    <row r="14" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R13" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
         <v>12</v>
       </c>
@@ -1274,8 +1332,11 @@
       <c r="K14">
         <v>1000</v>
       </c>
-    </row>
-    <row r="15" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R14" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
         <v>13</v>
       </c>
@@ -1312,8 +1373,11 @@
       <c r="L15">
         <v>500</v>
       </c>
-    </row>
-    <row r="16" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R15" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
         <v>14</v>
       </c>
@@ -1353,8 +1417,11 @@
       <c r="M16">
         <v>500</v>
       </c>
-    </row>
-    <row r="17" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R16" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
         <v>15</v>
       </c>
@@ -1403,8 +1470,11 @@
       <c r="P17">
         <v>100</v>
       </c>
-    </row>
-    <row r="18" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R17" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
         <v>16</v>
       </c>
@@ -1453,8 +1523,11 @@
       <c r="P18">
         <v>1000</v>
       </c>
-    </row>
-    <row r="19" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R18" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
         <v>17</v>
       </c>
@@ -1497,8 +1570,11 @@
       <c r="N19">
         <v>2000</v>
       </c>
-    </row>
-    <row r="20" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R19" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
         <v>18</v>
       </c>
@@ -1535,8 +1611,11 @@
       <c r="L20">
         <v>500</v>
       </c>
-    </row>
-    <row r="21" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R20" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
         <v>19</v>
       </c>
@@ -1576,8 +1655,11 @@
       <c r="M21">
         <v>1500</v>
       </c>
-    </row>
-    <row r="22" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R21" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
         <v>20</v>
       </c>
@@ -1617,8 +1699,11 @@
       <c r="M22">
         <v>1000</v>
       </c>
-    </row>
-    <row r="23" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R22" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
         <v>21</v>
       </c>
@@ -1661,8 +1746,11 @@
       <c r="N23">
         <v>500</v>
       </c>
-    </row>
-    <row r="24" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R23" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
         <v>22</v>
       </c>
@@ -1702,8 +1790,11 @@
       <c r="M24">
         <v>500</v>
       </c>
-    </row>
-    <row r="25" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R24" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
         <v>23</v>
       </c>
@@ -1746,8 +1837,11 @@
       <c r="N25">
         <v>1000</v>
       </c>
-    </row>
-    <row r="26" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R25" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
         <v>24</v>
       </c>
@@ -1796,8 +1890,11 @@
       <c r="P26">
         <v>1500</v>
       </c>
-    </row>
-    <row r="27" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R26" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
         <v>25</v>
       </c>
@@ -1837,8 +1934,11 @@
       <c r="M27">
         <v>1000</v>
       </c>
-    </row>
-    <row r="28" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R27" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
         <v>26</v>
       </c>
@@ -1884,8 +1984,11 @@
       <c r="O28">
         <v>1500</v>
       </c>
-    </row>
-    <row r="29" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R28" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
         <v>27</v>
       </c>
@@ -1925,8 +2028,11 @@
       <c r="M29">
         <v>500</v>
       </c>
-    </row>
-    <row r="30" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R29" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
         <v>28</v>
       </c>
@@ -1972,8 +2078,11 @@
       <c r="O30">
         <v>1500</v>
       </c>
-    </row>
-    <row r="31" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R30" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
         <v>29</v>
       </c>
@@ -2025,8 +2134,11 @@
       <c r="Q31">
         <v>2000</v>
       </c>
-    </row>
-    <row r="32" spans="1:17" x14ac:dyDescent="0.3">
+      <c r="R31" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
         <v>30</v>
       </c>
@@ -2063,8 +2175,11 @@
       <c r="L32">
         <v>1500</v>
       </c>
-    </row>
-    <row r="33" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R32" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
         <v>31</v>
       </c>
@@ -2104,8 +2219,11 @@
       <c r="M33">
         <v>1000</v>
       </c>
-    </row>
-    <row r="34" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R33" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
         <v>32</v>
       </c>
@@ -2145,8 +2263,11 @@
       <c r="M34">
         <v>1500</v>
       </c>
-    </row>
-    <row r="35" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R34" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
         <v>33</v>
       </c>
@@ -2186,8 +2307,11 @@
       <c r="M35">
         <v>1000</v>
       </c>
-    </row>
-    <row r="36" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R35" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
         <v>34</v>
       </c>
@@ -2227,8 +2351,12 @@
       <c r="M36">
         <v>1000</v>
       </c>
-    </row>
-    <row r="37" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R36" t="s">
+        <v>104</v>
+      </c>
+      <c r="T36" s="2"/>
+    </row>
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
         <v>35</v>
       </c>
@@ -2265,8 +2393,11 @@
       <c r="L37">
         <v>1000</v>
       </c>
-    </row>
-    <row r="38" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R37" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
         <v>36</v>
       </c>
@@ -2306,8 +2437,14 @@
       <c r="M38">
         <v>500</v>
       </c>
-    </row>
-    <row r="39" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R38" t="s">
+        <v>104</v>
+      </c>
+      <c r="T38" t="s">
+        <v>105</v>
+      </c>
+    </row>
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
         <v>37</v>
       </c>
@@ -2356,8 +2493,11 @@
       <c r="P39">
         <v>1500</v>
       </c>
-    </row>
-    <row r="40" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R39" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
         <v>38</v>
       </c>
@@ -2397,8 +2537,11 @@
       <c r="M40">
         <v>1400</v>
       </c>
-    </row>
-    <row r="41" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R40" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
         <v>39</v>
       </c>
@@ -2444,8 +2587,11 @@
       <c r="O41">
         <v>1500</v>
       </c>
-    </row>
-    <row r="42" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R41" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
         <v>40</v>
       </c>
@@ -2488,8 +2634,11 @@
       <c r="N42">
         <v>2000</v>
       </c>
-    </row>
-    <row r="43" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R42" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
         <v>41</v>
       </c>
@@ -2538,8 +2687,11 @@
       <c r="P43">
         <v>1000</v>
       </c>
-    </row>
-    <row r="44" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R43" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
         <v>42</v>
       </c>
@@ -2582,8 +2734,11 @@
       <c r="N44">
         <v>500</v>
       </c>
-    </row>
-    <row r="45" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R44" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
         <v>43</v>
       </c>
@@ -2629,8 +2784,11 @@
       <c r="O45">
         <v>1000</v>
       </c>
-    </row>
-    <row r="46" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R45" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
         <v>44</v>
       </c>
@@ -2673,8 +2831,11 @@
       <c r="N46">
         <v>1500</v>
       </c>
-    </row>
-    <row r="47" spans="1:16" x14ac:dyDescent="0.3">
+      <c r="R46" t="s">
+        <v>104</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
         <v>45</v>
       </c>
@@ -2701,10 +2862,16 @@
       </c>
       <c r="I47">
         <v>9000</v>
+      </c>
+      <c r="R47" t="s">
+        <v>104</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+  <ignoredErrors>
+    <ignoredError sqref="I1:Q1" numberStoredAsText="1"/>
+  </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Se termina la distribución de unidades por vueltas
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{97C80A4C-181C-4E3E-8880-D837BE074D63}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8C053A-924E-445C-8519-899E31D3DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="106">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="107">
   <si>
     <t>Placa de tracto</t>
   </si>
@@ -338,6 +338,9 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>NO</t>
   </si>
 </sst>
 </file>
@@ -711,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A22" workbookViewId="0">
-      <selection activeCell="T43" sqref="T43"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="T27" sqref="T27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1891,7 +1894,7 @@
         <v>1500</v>
       </c>
       <c r="R26" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
@@ -1935,7 +1938,7 @@
         <v>1000</v>
       </c>
       <c r="R27" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
@@ -1985,7 +1988,7 @@
         <v>1500</v>
       </c>
       <c r="R28" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
@@ -2029,7 +2032,7 @@
         <v>500</v>
       </c>
       <c r="R29" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
@@ -2079,7 +2082,7 @@
         <v>1500</v>
       </c>
       <c r="R30" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
@@ -2135,7 +2138,7 @@
         <v>2000</v>
       </c>
       <c r="R31" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
@@ -2176,7 +2179,7 @@
         <v>1500</v>
       </c>
       <c r="R32" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
@@ -2220,7 +2223,7 @@
         <v>1000</v>
       </c>
       <c r="R33" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
@@ -2264,7 +2267,7 @@
         <v>1500</v>
       </c>
       <c r="R34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
@@ -2308,7 +2311,7 @@
         <v>1000</v>
       </c>
       <c r="R35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -2352,7 +2355,7 @@
         <v>1000</v>
       </c>
       <c r="R36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="T36" s="2"/>
     </row>
@@ -2394,7 +2397,7 @@
         <v>1000</v>
       </c>
       <c r="R37" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
@@ -2438,7 +2441,7 @@
         <v>500</v>
       </c>
       <c r="R38" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="T38" t="s">
         <v>105</v>
@@ -2494,7 +2497,7 @@
         <v>1500</v>
       </c>
       <c r="R39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
@@ -2538,7 +2541,7 @@
         <v>1400</v>
       </c>
       <c r="R40" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
@@ -2588,7 +2591,7 @@
         <v>1500</v>
       </c>
       <c r="R41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
@@ -2635,7 +2638,7 @@
         <v>2000</v>
       </c>
       <c r="R42" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
@@ -2688,7 +2691,7 @@
         <v>1000</v>
       </c>
       <c r="R43" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
@@ -2735,7 +2738,7 @@
         <v>500</v>
       </c>
       <c r="R44" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
@@ -2785,7 +2788,7 @@
         <v>1000</v>
       </c>
       <c r="R45" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
@@ -2832,7 +2835,7 @@
         <v>1500</v>
       </c>
       <c r="R46" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
@@ -2864,7 +2867,7 @@
         <v>9000</v>
       </c>
       <c r="R47" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Se termina de mostrar las vueltas en el mapa
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D8C053A-924E-445C-8519-899E31D3DA4E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7C0687-D089-476D-B6E3-92AF6D890EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -714,8 +714,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="T27" sqref="T27"/>
+    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="T23" sqref="T23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1750,7 +1750,7 @@
         <v>500</v>
       </c>
       <c r="R23" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
@@ -1794,7 +1794,7 @@
         <v>500</v>
       </c>
       <c r="R24" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
@@ -1841,7 +1841,7 @@
         <v>1000</v>
       </c>
       <c r="R25" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">

</xml_diff>

<commit_message>
Restricciones de abastecer una vez por estación y recorrer máxmo tres estaciones por unidad terminadas
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -1,20 +1,23 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24701"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4B7C0687-D089-476D-B6E3-92AF6D890EE5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D418B37D-6A4A-45F8-8FA5-917A3E6922DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja 1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">'Hoja 1'!$A$1:$R$47</definedName>
+  </definedNames>
   <calcPr calcId="0"/>
 </workbook>
 </file>
@@ -714,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A7" workbookViewId="0">
-      <selection activeCell="T23" sqref="T23"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="T16" sqref="T16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1178,7 +1181,7 @@
         <v>1000</v>
       </c>
       <c r="R10" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
@@ -1257,7 +1260,7 @@
         <v>500</v>
       </c>
       <c r="R12" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
@@ -1377,7 +1380,7 @@
         <v>500</v>
       </c>
       <c r="R15" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
@@ -1615,7 +1618,7 @@
         <v>500</v>
       </c>
       <c r="R20" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
@@ -2267,7 +2270,7 @@
         <v>1500</v>
       </c>
       <c r="R34" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
@@ -2311,7 +2314,7 @@
         <v>1000</v>
       </c>
       <c r="R35" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
@@ -2355,7 +2358,7 @@
         <v>1000</v>
       </c>
       <c r="R36" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T36" s="2"/>
     </row>
@@ -2441,7 +2444,7 @@
         <v>500</v>
       </c>
       <c r="R38" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="T38" t="s">
         <v>105</v>
@@ -2871,6 +2874,9 @@
       </c>
     </row>
   </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R47">
+    <sortCondition ref="A1:A47"/>
+  </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
   <ignoredErrors>

</xml_diff>

<commit_message>
Se termina de agregar restricción de capacidad máxima por estación
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D418B37D-6A4A-45F8-8FA5-917A3E6922DA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541C3D8-4589-443D-A9F5-DE88F8647AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="T16" sqref="T16"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="S43" sqref="S43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,145 +790,160 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>0</v>
+        <v>38</v>
       </c>
       <c r="B2" t="s">
-        <v>16</v>
+        <v>85</v>
       </c>
       <c r="C2" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D2" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E2" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2">
-        <v>4000</v>
+        <v>10400</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="I2">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="J2">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="K2">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="L2">
         <v>1000</v>
       </c>
       <c r="M2">
-        <v>500</v>
+        <v>1400</v>
       </c>
       <c r="R2" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>1</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>64</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>18</v>
+        <v>65</v>
       </c>
       <c r="E3" t="s">
-        <v>22</v>
+        <v>66</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3">
-        <v>7500</v>
+        <v>10000</v>
       </c>
       <c r="H3">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I3">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="J3">
-        <v>1000</v>
+        <v>2500</v>
       </c>
       <c r="K3">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="L3">
         <v>1000</v>
       </c>
       <c r="M3">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N3">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="O3">
-        <v>500</v>
-      </c>
-      <c r="P3">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R3" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>2</v>
+        <v>29</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>70</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>18</v>
+        <v>71</v>
       </c>
       <c r="E4" t="s">
-        <v>24</v>
+        <v>72</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4">
-        <v>9000</v>
+        <v>10000</v>
       </c>
       <c r="H4">
-        <v>3</v>
+        <v>9</v>
       </c>
       <c r="I4">
-        <v>4000</v>
+        <v>2000</v>
       </c>
       <c r="J4">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="K4">
+        <v>1000</v>
+      </c>
+      <c r="L4">
+        <v>500</v>
+      </c>
+      <c r="M4">
+        <v>1000</v>
+      </c>
+      <c r="N4">
+        <v>500</v>
+      </c>
+      <c r="O4">
+        <v>1000</v>
+      </c>
+      <c r="P4">
+        <v>1000</v>
+      </c>
+      <c r="Q4">
         <v>2000</v>
       </c>
       <c r="R4" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>3</v>
+        <v>2</v>
       </c>
       <c r="B5" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -937,7 +952,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -946,10 +961,16 @@
         <v>9000</v>
       </c>
       <c r="H5">
-        <v>1</v>
+        <v>3</v>
       </c>
       <c r="I5">
-        <v>9000</v>
+        <v>4000</v>
+      </c>
+      <c r="J5">
+        <v>3000</v>
+      </c>
+      <c r="K5">
+        <v>2000</v>
       </c>
       <c r="R5" t="s">
         <v>104</v>
@@ -957,46 +978,31 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>4</v>
+        <v>3</v>
       </c>
       <c r="B6" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>28</v>
+        <v>18</v>
       </c>
       <c r="E6" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6">
-        <v>4500</v>
+        <v>9000</v>
       </c>
       <c r="H6">
-        <v>6</v>
+        <v>1</v>
       </c>
       <c r="I6">
-        <v>500</v>
-      </c>
-      <c r="J6">
-        <v>1000</v>
-      </c>
-      <c r="K6">
-        <v>1000</v>
-      </c>
-      <c r="L6">
-        <v>1000</v>
-      </c>
-      <c r="M6">
-        <v>500</v>
-      </c>
-      <c r="N6">
-        <v>500</v>
+        <v>9000</v>
       </c>
       <c r="R6" t="s">
         <v>104</v>
@@ -1004,49 +1010,37 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>5</v>
+        <v>9</v>
       </c>
       <c r="B7" t="s">
-        <v>29</v>
+        <v>36</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>28</v>
+        <v>34</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>37</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7">
-        <v>4500</v>
+        <v>9000</v>
       </c>
       <c r="H7">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I7">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="J7">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="K7">
-        <v>500</v>
-      </c>
-      <c r="L7">
-        <v>500</v>
-      </c>
-      <c r="M7">
-        <v>500</v>
-      </c>
-      <c r="N7">
-        <v>500</v>
-      </c>
-      <c r="O7">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="R7" t="s">
         <v>104</v>
@@ -1054,49 +1048,46 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
+        <v>17</v>
+      </c>
+      <c r="B8" t="s">
+        <v>50</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>51</v>
+      </c>
+      <c r="E8" t="s">
+        <v>52</v>
+      </c>
+      <c r="F8" t="s">
+        <v>20</v>
+      </c>
+      <c r="G8">
+        <v>9000</v>
+      </c>
+      <c r="H8">
         <v>6</v>
       </c>
-      <c r="B8" t="s">
-        <v>30</v>
-      </c>
-      <c r="C8" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" t="s">
-        <v>31</v>
-      </c>
-      <c r="E8" t="s">
-        <v>32</v>
-      </c>
-      <c r="F8" t="s">
-        <v>20</v>
-      </c>
-      <c r="G8">
-        <v>6000</v>
-      </c>
-      <c r="H8">
-        <v>7</v>
-      </c>
       <c r="I8">
+        <v>2000</v>
+      </c>
+      <c r="J8">
         <v>1500</v>
       </c>
-      <c r="J8">
-        <v>1000</v>
-      </c>
       <c r="K8">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L8">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M8">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="N8">
-        <v>1000</v>
-      </c>
-      <c r="O8">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="R8" t="s">
         <v>104</v>
@@ -1104,81 +1095,102 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>7</v>
+        <v>24</v>
       </c>
       <c r="B9" t="s">
-        <v>33</v>
+        <v>61</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>34</v>
+        <v>59</v>
       </c>
       <c r="E9" t="s">
-        <v>19</v>
+        <v>62</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
       <c r="G9">
-        <v>6500</v>
+        <v>9000</v>
       </c>
       <c r="H9">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I9">
-        <v>2500</v>
+        <v>2000</v>
       </c>
       <c r="J9">
+        <v>1000</v>
+      </c>
+      <c r="K9">
+        <v>500</v>
+      </c>
+      <c r="L9">
+        <v>1000</v>
+      </c>
+      <c r="M9">
+        <v>1000</v>
+      </c>
+      <c r="N9">
         <v>1500</v>
       </c>
-      <c r="K9">
-        <v>1000</v>
-      </c>
-      <c r="L9">
+      <c r="O9">
+        <v>500</v>
+      </c>
+      <c r="P9">
         <v>1500</v>
       </c>
       <c r="R9" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B10" t="s">
-        <v>35</v>
+        <v>68</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>34</v>
+        <v>65</v>
       </c>
       <c r="E10" t="s">
-        <v>19</v>
+        <v>69</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
       <c r="G10">
-        <v>3500</v>
+        <v>9000</v>
       </c>
       <c r="H10">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I10">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="J10">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K10">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L10">
-        <v>1000</v>
+        <v>500</v>
+      </c>
+      <c r="M10">
+        <v>1000</v>
+      </c>
+      <c r="N10">
+        <v>1500</v>
+      </c>
+      <c r="O10">
+        <v>1500</v>
       </c>
       <c r="R10" t="s">
         <v>106</v>
@@ -1186,19 +1198,19 @@
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
-        <v>9</v>
+        <v>37</v>
       </c>
       <c r="B11" t="s">
-        <v>36</v>
+        <v>83</v>
       </c>
       <c r="C11" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D11" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E11" t="s">
-        <v>37</v>
+        <v>84</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1207,57 +1219,78 @@
         <v>9000</v>
       </c>
       <c r="H11">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="I11">
-        <v>3000</v>
+        <v>2000</v>
       </c>
       <c r="J11">
-        <v>3000</v>
+        <v>1500</v>
       </c>
       <c r="K11">
-        <v>3000</v>
+        <v>1000</v>
+      </c>
+      <c r="L11">
+        <v>500</v>
+      </c>
+      <c r="M11">
+        <v>500</v>
+      </c>
+      <c r="N11">
+        <v>1000</v>
+      </c>
+      <c r="O11">
+        <v>1000</v>
+      </c>
+      <c r="P11">
+        <v>1500</v>
       </c>
       <c r="R11" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
-        <v>10</v>
+        <v>40</v>
       </c>
       <c r="B12" t="s">
-        <v>38</v>
+        <v>89</v>
       </c>
       <c r="C12" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D12" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E12" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="F12" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G12">
-        <v>3000</v>
+        <v>9000</v>
       </c>
       <c r="H12">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I12">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J12">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K12">
         <v>1000</v>
       </c>
       <c r="L12">
-        <v>500</v>
+        <v>1000</v>
+      </c>
+      <c r="M12">
+        <v>1500</v>
+      </c>
+      <c r="N12">
+        <v>2000</v>
       </c>
       <c r="R12" t="s">
         <v>106</v>
@@ -1265,31 +1298,31 @@
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>11</v>
+        <v>44</v>
       </c>
       <c r="B13" t="s">
-        <v>40</v>
+        <v>99</v>
       </c>
       <c r="C13" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D13" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E13" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F13" t="s">
         <v>20</v>
       </c>
       <c r="G13">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="H13">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I13">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J13">
         <v>1000</v>
@@ -1298,118 +1331,130 @@
         <v>1000</v>
       </c>
       <c r="L13">
+        <v>2000</v>
+      </c>
+      <c r="M13">
         <v>1500</v>
       </c>
+      <c r="N13">
+        <v>1500</v>
+      </c>
       <c r="R13" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>12</v>
+        <v>45</v>
       </c>
       <c r="B14" t="s">
-        <v>41</v>
+        <v>101</v>
       </c>
       <c r="C14" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D14" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E14" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="F14" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G14">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="H14">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I14">
-        <v>2000</v>
-      </c>
-      <c r="J14">
-        <v>1000</v>
-      </c>
-      <c r="K14">
-        <v>1000</v>
+        <v>9000</v>
       </c>
       <c r="R14" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>13</v>
+        <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>42</v>
+        <v>46</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
       </c>
       <c r="D15" t="s">
-        <v>34</v>
+        <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>43</v>
+        <v>47</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15">
-        <v>3500</v>
+        <v>7600</v>
       </c>
       <c r="H15">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="I15">
         <v>2000</v>
       </c>
       <c r="J15">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K15">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L15">
         <v>500</v>
       </c>
+      <c r="M15">
+        <v>500</v>
+      </c>
+      <c r="N15">
+        <v>1000</v>
+      </c>
+      <c r="O15">
+        <v>1000</v>
+      </c>
+      <c r="P15">
+        <v>100</v>
+      </c>
       <c r="R15" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>14</v>
+        <v>1</v>
       </c>
       <c r="B16" t="s">
-        <v>44</v>
+        <v>21</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="E16" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16">
-        <v>4000</v>
+        <v>7500</v>
       </c>
       <c r="H16">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I16">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J16">
         <v>1000</v>
@@ -1422,6 +1467,15 @@
       </c>
       <c r="M16">
         <v>500</v>
+      </c>
+      <c r="N16">
+        <v>500</v>
+      </c>
+      <c r="O16">
+        <v>500</v>
+      </c>
+      <c r="P16">
+        <v>1000</v>
       </c>
       <c r="R16" t="s">
         <v>104</v>
@@ -1429,10 +1483,10 @@
     </row>
     <row r="17" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A17" s="1">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B17" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="C17" t="s">
         <v>17</v>
@@ -1441,13 +1495,13 @@
         <v>45</v>
       </c>
       <c r="E17" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
       <c r="F17" t="s">
         <v>20</v>
       </c>
       <c r="G17">
-        <v>7600</v>
+        <v>7500</v>
       </c>
       <c r="H17">
         <v>8</v>
@@ -1456,16 +1510,16 @@
         <v>2000</v>
       </c>
       <c r="J17">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K17">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L17">
         <v>500</v>
       </c>
       <c r="M17">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N17">
         <v>1000</v>
@@ -1474,7 +1528,7 @@
         <v>1000</v>
       </c>
       <c r="P17">
-        <v>100</v>
+        <v>1000</v>
       </c>
       <c r="R17" t="s">
         <v>104</v>
@@ -1482,19 +1536,19 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>16</v>
+        <v>39</v>
       </c>
       <c r="B18" t="s">
-        <v>48</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D18" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="E18" t="s">
-        <v>49</v>
+        <v>88</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
@@ -1503,13 +1557,13 @@
         <v>7500</v>
       </c>
       <c r="H18">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="I18">
         <v>2000</v>
       </c>
       <c r="J18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K18">
         <v>500</v>
@@ -1518,80 +1572,83 @@
         <v>500</v>
       </c>
       <c r="M18">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N18">
         <v>1000</v>
       </c>
       <c r="O18">
-        <v>1000</v>
-      </c>
-      <c r="P18">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R18" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>17</v>
+        <v>41</v>
       </c>
       <c r="B19" t="s">
-        <v>50</v>
+        <v>91</v>
       </c>
       <c r="C19" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D19" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="E19" t="s">
-        <v>52</v>
+        <v>94</v>
       </c>
       <c r="F19" t="s">
         <v>20</v>
       </c>
       <c r="G19">
-        <v>9000</v>
+        <v>7500</v>
       </c>
       <c r="H19">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="I19">
         <v>2000</v>
       </c>
       <c r="J19">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K19">
         <v>1000</v>
       </c>
       <c r="L19">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M19">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="N19">
-        <v>2000</v>
+        <v>500</v>
+      </c>
+      <c r="O19">
+        <v>1000</v>
+      </c>
+      <c r="P19">
+        <v>1000</v>
       </c>
       <c r="R19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>18</v>
+        <v>7</v>
       </c>
       <c r="B20" t="s">
-        <v>53</v>
+        <v>33</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>51</v>
+        <v>34</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -1600,66 +1657,72 @@
         <v>20</v>
       </c>
       <c r="G20">
-        <v>2500</v>
+        <v>6500</v>
       </c>
       <c r="H20">
         <v>4</v>
       </c>
       <c r="I20">
-        <v>500</v>
+        <v>2500</v>
       </c>
       <c r="J20">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K20">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L20">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="R20" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>19</v>
+        <v>6</v>
       </c>
       <c r="B21" t="s">
-        <v>54</v>
+        <v>30</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E21" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="F21" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G21">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H21">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I21">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="J21">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K21">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L21">
         <v>500</v>
       </c>
       <c r="M21">
-        <v>1500</v>
+        <v>500</v>
+      </c>
+      <c r="N21">
+        <v>1000</v>
+      </c>
+      <c r="O21">
+        <v>1000</v>
       </c>
       <c r="R21" t="s">
         <v>104</v>
@@ -1667,34 +1730,34 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>20</v>
+        <v>42</v>
       </c>
       <c r="B22" t="s">
-        <v>55</v>
+        <v>95</v>
       </c>
       <c r="C22" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D22" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="E22" t="s">
-        <v>19</v>
+        <v>96</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
       <c r="G22">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H22">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I22">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="J22">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K22">
         <v>1000</v>
@@ -1703,54 +1766,60 @@
         <v>1000</v>
       </c>
       <c r="M22">
-        <v>1000</v>
+        <v>500</v>
+      </c>
+      <c r="N22">
+        <v>500</v>
       </c>
       <c r="R22" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>21</v>
+        <v>43</v>
       </c>
       <c r="B23" t="s">
-        <v>56</v>
+        <v>97</v>
       </c>
       <c r="C23" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D23" t="s">
-        <v>57</v>
+        <v>93</v>
       </c>
       <c r="E23" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23">
-        <v>4000</v>
+        <v>6000</v>
       </c>
       <c r="H23">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I23">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="J23">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K23">
         <v>500</v>
       </c>
       <c r="L23">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M23">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N23">
-        <v>500</v>
+        <v>1000</v>
+      </c>
+      <c r="O23">
+        <v>1000</v>
       </c>
       <c r="R23" t="s">
         <v>106</v>
@@ -1758,16 +1827,16 @@
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>22</v>
+        <v>4</v>
       </c>
       <c r="B24" t="s">
-        <v>58</v>
+        <v>27</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E24" t="s">
         <v>19</v>
@@ -1776,10 +1845,10 @@
         <v>20</v>
       </c>
       <c r="G24">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="H24">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I24">
         <v>500</v>
@@ -1796,22 +1865,25 @@
       <c r="M24">
         <v>500</v>
       </c>
+      <c r="N24">
+        <v>500</v>
+      </c>
       <c r="R24" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>23</v>
+        <v>5</v>
       </c>
       <c r="B25" t="s">
-        <v>60</v>
+        <v>29</v>
       </c>
       <c r="C25" t="s">
         <v>17</v>
       </c>
       <c r="D25" t="s">
-        <v>59</v>
+        <v>28</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -1820,13 +1892,13 @@
         <v>20</v>
       </c>
       <c r="G25">
-        <v>4000</v>
+        <v>4500</v>
       </c>
       <c r="H25">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I25">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J25">
         <v>500</v>
@@ -1838,80 +1910,74 @@
         <v>500</v>
       </c>
       <c r="M25">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N25">
+        <v>500</v>
+      </c>
+      <c r="O25">
         <v>1000</v>
       </c>
       <c r="R25" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="B26" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="C26" t="s">
         <v>17</v>
       </c>
       <c r="D26" t="s">
-        <v>59</v>
+        <v>18</v>
       </c>
       <c r="E26" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F26" t="s">
         <v>20</v>
       </c>
       <c r="G26">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H26">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I26">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J26">
         <v>1000</v>
       </c>
       <c r="K26">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L26">
         <v>1000</v>
       </c>
       <c r="M26">
-        <v>1000</v>
-      </c>
-      <c r="N26">
-        <v>1500</v>
-      </c>
-      <c r="O26">
-        <v>500</v>
-      </c>
-      <c r="P26">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="R26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="B27" t="s">
-        <v>63</v>
+        <v>40</v>
       </c>
       <c r="C27" t="s">
         <v>17</v>
       </c>
       <c r="D27" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -1923,89 +1989,74 @@
         <v>4000</v>
       </c>
       <c r="H27">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I27">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J27">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K27">
         <v>1000</v>
       </c>
       <c r="L27">
-        <v>500</v>
-      </c>
-      <c r="M27">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R27" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>26</v>
+        <v>12</v>
       </c>
       <c r="B28" t="s">
-        <v>64</v>
+        <v>41</v>
       </c>
       <c r="C28" t="s">
         <v>17</v>
       </c>
       <c r="D28" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E28" t="s">
-        <v>66</v>
+        <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G28">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="H28">
-        <v>7</v>
+        <v>3</v>
       </c>
       <c r="I28">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J28">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="K28">
-        <v>1500</v>
-      </c>
-      <c r="L28">
-        <v>1000</v>
-      </c>
-      <c r="M28">
-        <v>1000</v>
-      </c>
-      <c r="N28">
-        <v>1500</v>
-      </c>
-      <c r="O28">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="R28" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="B29" t="s">
-        <v>67</v>
+        <v>44</v>
       </c>
       <c r="C29" t="s">
         <v>17</v>
       </c>
       <c r="D29" t="s">
-        <v>65</v>
+        <v>45</v>
       </c>
       <c r="E29" t="s">
         <v>19</v>
@@ -2020,10 +2071,10 @@
         <v>5</v>
       </c>
       <c r="I29">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J29">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K29">
         <v>1000</v>
@@ -2035,127 +2086,109 @@
         <v>500</v>
       </c>
       <c r="R29" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>28</v>
+        <v>19</v>
       </c>
       <c r="B30" t="s">
-        <v>68</v>
+        <v>54</v>
       </c>
       <c r="C30" t="s">
         <v>17</v>
       </c>
       <c r="D30" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="E30" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="F30" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G30">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H30">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I30">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="J30">
+        <v>500</v>
+      </c>
+      <c r="K30">
+        <v>1000</v>
+      </c>
+      <c r="L30">
+        <v>500</v>
+      </c>
+      <c r="M30">
         <v>1500</v>
       </c>
-      <c r="K30">
-        <v>500</v>
-      </c>
-      <c r="L30">
-        <v>500</v>
-      </c>
-      <c r="M30">
-        <v>1000</v>
-      </c>
-      <c r="N30">
-        <v>1500</v>
-      </c>
-      <c r="O30">
-        <v>1500</v>
-      </c>
       <c r="R30" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="B31" t="s">
-        <v>70</v>
+        <v>55</v>
       </c>
       <c r="C31" t="s">
         <v>17</v>
       </c>
       <c r="D31" t="s">
-        <v>71</v>
+        <v>51</v>
       </c>
       <c r="E31" t="s">
-        <v>72</v>
+        <v>19</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
       <c r="G31">
-        <v>10000</v>
+        <v>4000</v>
       </c>
       <c r="H31">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="I31">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J31">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K31">
         <v>1000</v>
       </c>
       <c r="L31">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M31">
         <v>1000</v>
       </c>
-      <c r="N31">
-        <v>500</v>
-      </c>
-      <c r="O31">
-        <v>1000</v>
-      </c>
-      <c r="P31">
-        <v>1000</v>
-      </c>
-      <c r="Q31">
-        <v>2000</v>
-      </c>
       <c r="R31" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>30</v>
+        <v>21</v>
       </c>
       <c r="B32" t="s">
-        <v>73</v>
+        <v>56</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>74</v>
+        <v>57</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
@@ -2167,19 +2200,25 @@
         <v>4000</v>
       </c>
       <c r="H32">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I32">
         <v>500</v>
       </c>
       <c r="J32">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K32">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L32">
-        <v>1500</v>
+        <v>1000</v>
+      </c>
+      <c r="M32">
+        <v>1000</v>
+      </c>
+      <c r="N32">
+        <v>500</v>
       </c>
       <c r="R32" t="s">
         <v>106</v>
@@ -2187,16 +2226,16 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>31</v>
+        <v>22</v>
       </c>
       <c r="B33" t="s">
-        <v>75</v>
+        <v>58</v>
       </c>
       <c r="C33" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
@@ -2211,19 +2250,19 @@
         <v>5</v>
       </c>
       <c r="I33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J33">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K33">
         <v>1000</v>
       </c>
       <c r="L33">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R33" t="s">
         <v>106</v>
@@ -2231,16 +2270,16 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>32</v>
+        <v>23</v>
       </c>
       <c r="B34" t="s">
-        <v>78</v>
+        <v>60</v>
       </c>
       <c r="C34" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -2252,10 +2291,10 @@
         <v>4000</v>
       </c>
       <c r="H34">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I34">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J34">
         <v>500</v>
@@ -2267,24 +2306,27 @@
         <v>500</v>
       </c>
       <c r="M34">
-        <v>1500</v>
+        <v>1000</v>
+      </c>
+      <c r="N34">
+        <v>1000</v>
       </c>
       <c r="R34" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>33</v>
+        <v>25</v>
       </c>
       <c r="B35" t="s">
-        <v>79</v>
+        <v>63</v>
       </c>
       <c r="C35" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D35" t="s">
-        <v>77</v>
+        <v>59</v>
       </c>
       <c r="E35" t="s">
         <v>19</v>
@@ -2314,21 +2356,21 @@
         <v>1000</v>
       </c>
       <c r="R35" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>34</v>
+        <v>27</v>
       </c>
       <c r="B36" t="s">
-        <v>80</v>
+        <v>67</v>
       </c>
       <c r="C36" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -2343,37 +2385,37 @@
         <v>5</v>
       </c>
       <c r="I36">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J36">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K36">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L36">
         <v>1000</v>
       </c>
       <c r="M36">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R36" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="T36" s="2"/>
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>35</v>
+        <v>30</v>
       </c>
       <c r="B37" t="s">
-        <v>81</v>
+        <v>73</v>
       </c>
       <c r="C37" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -2382,22 +2424,22 @@
         <v>20</v>
       </c>
       <c r="G37">
-        <v>3000</v>
+        <v>4000</v>
       </c>
       <c r="H37">
         <v>4</v>
       </c>
       <c r="I37">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J37">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K37">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L37">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R37" t="s">
         <v>106</v>
@@ -2405,10 +2447,10 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="B38" t="s">
-        <v>82</v>
+        <v>75</v>
       </c>
       <c r="C38" t="s">
         <v>76</v>
@@ -2429,22 +2471,22 @@
         <v>5</v>
       </c>
       <c r="I38">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J38">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K38">
         <v>1000</v>
       </c>
       <c r="L38">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M38">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="R38" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="T38" t="s">
         <v>105</v>
@@ -2452,10 +2494,10 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>37</v>
+        <v>32</v>
       </c>
       <c r="B39" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C39" t="s">
         <v>76</v>
@@ -2464,51 +2506,42 @@
         <v>77</v>
       </c>
       <c r="E39" t="s">
-        <v>84</v>
+        <v>19</v>
       </c>
       <c r="F39" t="s">
         <v>20</v>
       </c>
       <c r="G39">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H39">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I39">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="J39">
+        <v>500</v>
+      </c>
+      <c r="K39">
+        <v>500</v>
+      </c>
+      <c r="L39">
+        <v>500</v>
+      </c>
+      <c r="M39">
         <v>1500</v>
       </c>
-      <c r="K39">
-        <v>1000</v>
-      </c>
-      <c r="L39">
-        <v>500</v>
-      </c>
-      <c r="M39">
-        <v>500</v>
-      </c>
-      <c r="N39">
-        <v>1000</v>
-      </c>
-      <c r="O39">
-        <v>1000</v>
-      </c>
-      <c r="P39">
-        <v>1500</v>
-      </c>
       <c r="R39" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>38</v>
+        <v>33</v>
       </c>
       <c r="B40" t="s">
-        <v>85</v>
+        <v>79</v>
       </c>
       <c r="C40" t="s">
         <v>76</v>
@@ -2517,42 +2550,42 @@
         <v>77</v>
       </c>
       <c r="E40" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="F40" t="s">
         <v>20</v>
       </c>
       <c r="G40">
-        <v>10400</v>
+        <v>4000</v>
       </c>
       <c r="H40">
         <v>5</v>
       </c>
       <c r="I40">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="J40">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="K40">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="L40">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M40">
-        <v>1400</v>
+        <v>1000</v>
       </c>
       <c r="R40" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>39</v>
+        <v>34</v>
       </c>
       <c r="B41" t="s">
-        <v>87</v>
+        <v>80</v>
       </c>
       <c r="C41" t="s">
         <v>76</v>
@@ -2561,48 +2594,42 @@
         <v>77</v>
       </c>
       <c r="E41" t="s">
-        <v>88</v>
+        <v>19</v>
       </c>
       <c r="F41" t="s">
         <v>20</v>
       </c>
       <c r="G41">
-        <v>7500</v>
+        <v>4000</v>
       </c>
       <c r="H41">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I41">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J41">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K41">
         <v>500</v>
       </c>
       <c r="L41">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M41">
-        <v>500</v>
-      </c>
-      <c r="N41">
-        <v>1000</v>
-      </c>
-      <c r="O41">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="R41" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>40</v>
+        <v>36</v>
       </c>
       <c r="B42" t="s">
-        <v>89</v>
+        <v>82</v>
       </c>
       <c r="C42" t="s">
         <v>76</v>
@@ -2611,22 +2638,22 @@
         <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
       </c>
       <c r="G42">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H42">
-        <v>6</v>
+        <v>5</v>
       </c>
       <c r="I42">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J42">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K42">
         <v>1000</v>
@@ -2635,160 +2662,130 @@
         <v>1000</v>
       </c>
       <c r="M42">
-        <v>1500</v>
-      </c>
-      <c r="N42">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="R42" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
-        <v>41</v>
+        <v>8</v>
       </c>
       <c r="B43" t="s">
-        <v>91</v>
+        <v>35</v>
       </c>
       <c r="C43" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D43" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="E43" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="F43" t="s">
         <v>20</v>
       </c>
       <c r="G43">
-        <v>7500</v>
+        <v>3500</v>
       </c>
       <c r="H43">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I43">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J43">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K43">
         <v>1000</v>
       </c>
       <c r="L43">
-        <v>500</v>
-      </c>
-      <c r="M43">
-        <v>1000</v>
-      </c>
-      <c r="N43">
-        <v>500</v>
-      </c>
-      <c r="O43">
-        <v>1000</v>
-      </c>
-      <c r="P43">
         <v>1000</v>
       </c>
       <c r="R43" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
+        <v>13</v>
+      </c>
+      <c r="B44" t="s">
         <v>42</v>
       </c>
-      <c r="B44" t="s">
-        <v>95</v>
-      </c>
       <c r="C44" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D44" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="E44" t="s">
-        <v>96</v>
+        <v>43</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
       </c>
       <c r="G44">
-        <v>6000</v>
+        <v>3500</v>
       </c>
       <c r="H44">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I44">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="J44">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K44">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L44">
-        <v>1000</v>
-      </c>
-      <c r="M44">
-        <v>500</v>
-      </c>
-      <c r="N44">
         <v>500</v>
       </c>
       <c r="R44" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>43</v>
+        <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>97</v>
+        <v>38</v>
       </c>
       <c r="C45" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D45" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="E45" t="s">
-        <v>98</v>
+        <v>19</v>
       </c>
       <c r="F45" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G45">
-        <v>6000</v>
+        <v>3000</v>
       </c>
       <c r="H45">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I45">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="J45">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K45">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L45">
         <v>500</v>
-      </c>
-      <c r="M45">
-        <v>500</v>
-      </c>
-      <c r="N45">
-        <v>1000</v>
-      </c>
-      <c r="O45">
-        <v>1000</v>
       </c>
       <c r="R45" t="s">
         <v>106</v>
@@ -2796,46 +2793,40 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>44</v>
+        <v>35</v>
       </c>
       <c r="B46" t="s">
-        <v>99</v>
+        <v>81</v>
       </c>
       <c r="C46" t="s">
-        <v>92</v>
+        <v>76</v>
       </c>
       <c r="D46" t="s">
-        <v>93</v>
+        <v>77</v>
       </c>
       <c r="E46" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
       </c>
       <c r="G46">
-        <v>9000</v>
+        <v>3000</v>
       </c>
       <c r="H46">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I46">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="J46">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K46">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L46">
-        <v>2000</v>
-      </c>
-      <c r="M46">
-        <v>1500</v>
-      </c>
-      <c r="N46">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="R46" t="s">
         <v>106</v>
@@ -2843,37 +2834,51 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>45</v>
+        <v>18</v>
       </c>
       <c r="B47" t="s">
-        <v>101</v>
+        <v>53</v>
       </c>
       <c r="C47" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D47" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E47" t="s">
-        <v>102</v>
+        <v>19</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
       <c r="G47">
-        <v>9000</v>
+        <v>2500</v>
       </c>
       <c r="H47">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I47">
-        <v>9000</v>
+        <v>500</v>
+      </c>
+      <c r="J47">
+        <v>1000</v>
+      </c>
+      <c r="K47">
+        <v>500</v>
+      </c>
+      <c r="L47">
+        <v>500</v>
       </c>
       <c r="R47" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
+  <autoFilter ref="A1:R47" xr:uid="{00000000-0001-0000-0000-000000000000}">
+    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R47">
+      <sortCondition descending="1" ref="G1:G47"/>
+    </sortState>
+  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R47">
     <sortCondition ref="A1:A47"/>
   </sortState>

</xml_diff>

<commit_message>
Se agrega restricción de detener la programación cuando ya no se pueda abastecer ninguna otra estación
</commit_message>
<xml_diff>
--- a/datos_entrada/Detalle_Unidades.xlsx
+++ b/datos_entrada/Detalle_Unidades.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\piero\Downloads\Optimizacion_Programacion\datos_entrada\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9541C3D8-4589-443D-A9F5-DE88F8647AF1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71258F01-66D7-49BA-8F32-51C2ABE2409F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -717,8 +717,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:T47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
-      <selection activeCell="S43" sqref="S43"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="S7" sqref="S7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -790,160 +790,145 @@
     </row>
     <row r="2" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A2" s="1">
-        <v>38</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>85</v>
+        <v>16</v>
       </c>
       <c r="C2" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D2" t="s">
-        <v>77</v>
+        <v>18</v>
       </c>
       <c r="E2" t="s">
-        <v>86</v>
+        <v>19</v>
       </c>
       <c r="F2" t="s">
         <v>20</v>
       </c>
       <c r="G2">
-        <v>10400</v>
+        <v>4000</v>
       </c>
       <c r="H2">
         <v>5</v>
       </c>
       <c r="I2">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="J2">
-        <v>2000</v>
+        <v>1000</v>
       </c>
       <c r="K2">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="L2">
         <v>1000</v>
       </c>
       <c r="M2">
-        <v>1400</v>
+        <v>500</v>
       </c>
       <c r="R2" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="3" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A3" s="1">
-        <v>26</v>
+        <v>1</v>
       </c>
       <c r="B3" t="s">
-        <v>64</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
         <v>17</v>
       </c>
       <c r="D3" t="s">
-        <v>65</v>
+        <v>18</v>
       </c>
       <c r="E3" t="s">
-        <v>66</v>
+        <v>22</v>
       </c>
       <c r="F3" t="s">
         <v>20</v>
       </c>
       <c r="G3">
-        <v>10000</v>
+        <v>7500</v>
       </c>
       <c r="H3">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I3">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J3">
-        <v>2500</v>
+        <v>1000</v>
       </c>
       <c r="K3">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="L3">
         <v>1000</v>
       </c>
       <c r="M3">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="N3">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="O3">
-        <v>1500</v>
+        <v>500</v>
+      </c>
+      <c r="P3">
+        <v>1000</v>
       </c>
       <c r="R3" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="4" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A4" s="1">
-        <v>29</v>
+        <v>2</v>
       </c>
       <c r="B4" t="s">
-        <v>70</v>
+        <v>23</v>
       </c>
       <c r="C4" t="s">
         <v>17</v>
       </c>
       <c r="D4" t="s">
-        <v>71</v>
+        <v>18</v>
       </c>
       <c r="E4" t="s">
-        <v>72</v>
+        <v>24</v>
       </c>
       <c r="F4" t="s">
         <v>20</v>
       </c>
       <c r="G4">
-        <v>10000</v>
+        <v>9000</v>
       </c>
       <c r="H4">
-        <v>9</v>
+        <v>3</v>
       </c>
       <c r="I4">
+        <v>4000</v>
+      </c>
+      <c r="J4">
+        <v>3000</v>
+      </c>
+      <c r="K4">
         <v>2000</v>
       </c>
-      <c r="J4">
-        <v>1000</v>
-      </c>
-      <c r="K4">
-        <v>1000</v>
-      </c>
-      <c r="L4">
-        <v>500</v>
-      </c>
-      <c r="M4">
-        <v>1000</v>
-      </c>
-      <c r="N4">
-        <v>500</v>
-      </c>
-      <c r="O4">
-        <v>1000</v>
-      </c>
-      <c r="P4">
-        <v>1000</v>
-      </c>
-      <c r="Q4">
-        <v>2000</v>
-      </c>
       <c r="R4" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="5" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A5" s="1">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="C5" t="s">
         <v>17</v>
@@ -952,7 +937,7 @@
         <v>18</v>
       </c>
       <c r="E5" t="s">
-        <v>24</v>
+        <v>26</v>
       </c>
       <c r="F5" t="s">
         <v>20</v>
@@ -961,16 +946,10 @@
         <v>9000</v>
       </c>
       <c r="H5">
-        <v>3</v>
+        <v>1</v>
       </c>
       <c r="I5">
-        <v>4000</v>
-      </c>
-      <c r="J5">
-        <v>3000</v>
-      </c>
-      <c r="K5">
-        <v>2000</v>
+        <v>9000</v>
       </c>
       <c r="R5" t="s">
         <v>104</v>
@@ -978,31 +957,46 @@
     </row>
     <row r="6" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A6" s="1">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="B6" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="C6" t="s">
         <v>17</v>
       </c>
       <c r="D6" t="s">
-        <v>18</v>
+        <v>28</v>
       </c>
       <c r="E6" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
       <c r="F6" t="s">
         <v>20</v>
       </c>
       <c r="G6">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="H6">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="I6">
-        <v>9000</v>
+        <v>500</v>
+      </c>
+      <c r="J6">
+        <v>1000</v>
+      </c>
+      <c r="K6">
+        <v>1000</v>
+      </c>
+      <c r="L6">
+        <v>1000</v>
+      </c>
+      <c r="M6">
+        <v>500</v>
+      </c>
+      <c r="N6">
+        <v>500</v>
       </c>
       <c r="R6" t="s">
         <v>104</v>
@@ -1010,37 +1004,49 @@
     </row>
     <row r="7" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A7" s="1">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="C7" t="s">
         <v>17</v>
       </c>
       <c r="D7" t="s">
-        <v>34</v>
+        <v>28</v>
       </c>
       <c r="E7" t="s">
-        <v>37</v>
+        <v>19</v>
       </c>
       <c r="F7" t="s">
         <v>20</v>
       </c>
       <c r="G7">
-        <v>9000</v>
+        <v>4500</v>
       </c>
       <c r="H7">
-        <v>3</v>
+        <v>7</v>
       </c>
       <c r="I7">
-        <v>3000</v>
+        <v>1000</v>
       </c>
       <c r="J7">
-        <v>3000</v>
+        <v>500</v>
       </c>
       <c r="K7">
-        <v>3000</v>
+        <v>500</v>
+      </c>
+      <c r="L7">
+        <v>500</v>
+      </c>
+      <c r="M7">
+        <v>500</v>
+      </c>
+      <c r="N7">
+        <v>500</v>
+      </c>
+      <c r="O7">
+        <v>1000</v>
       </c>
       <c r="R7" t="s">
         <v>104</v>
@@ -1048,46 +1054,49 @@
     </row>
     <row r="8" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A8" s="1">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="B8" t="s">
-        <v>50</v>
+        <v>30</v>
       </c>
       <c r="C8" t="s">
         <v>17</v>
       </c>
       <c r="D8" t="s">
-        <v>51</v>
+        <v>31</v>
       </c>
       <c r="E8" t="s">
-        <v>52</v>
+        <v>32</v>
       </c>
       <c r="F8" t="s">
         <v>20</v>
       </c>
       <c r="G8">
-        <v>9000</v>
+        <v>6000</v>
       </c>
       <c r="H8">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I8">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="J8">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L8">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M8">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="N8">
-        <v>2000</v>
+        <v>1000</v>
+      </c>
+      <c r="O8">
+        <v>1000</v>
       </c>
       <c r="R8" t="s">
         <v>104</v>
@@ -1095,122 +1104,101 @@
     </row>
     <row r="9" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A9" s="1">
-        <v>24</v>
+        <v>7</v>
       </c>
       <c r="B9" t="s">
-        <v>61</v>
+        <v>33</v>
       </c>
       <c r="C9" t="s">
         <v>17</v>
       </c>
       <c r="D9" t="s">
-        <v>59</v>
+        <v>34</v>
       </c>
       <c r="E9" t="s">
-        <v>62</v>
+        <v>19</v>
       </c>
       <c r="F9" t="s">
         <v>20</v>
       </c>
       <c r="G9">
-        <v>9000</v>
+        <v>6500</v>
       </c>
       <c r="H9">
-        <v>8</v>
+        <v>4</v>
       </c>
       <c r="I9">
-        <v>2000</v>
+        <v>2500</v>
       </c>
       <c r="J9">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K9">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L9">
-        <v>1000</v>
-      </c>
-      <c r="M9">
-        <v>1000</v>
-      </c>
-      <c r="N9">
         <v>1500</v>
       </c>
-      <c r="O9">
-        <v>500</v>
-      </c>
-      <c r="P9">
-        <v>1500</v>
-      </c>
       <c r="R9" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="10" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A10" s="1">
-        <v>28</v>
+        <v>8</v>
       </c>
       <c r="B10" t="s">
-        <v>68</v>
+        <v>35</v>
       </c>
       <c r="C10" t="s">
         <v>17</v>
       </c>
       <c r="D10" t="s">
-        <v>65</v>
+        <v>34</v>
       </c>
       <c r="E10" t="s">
-        <v>69</v>
+        <v>19</v>
       </c>
       <c r="F10" t="s">
         <v>20</v>
       </c>
       <c r="G10">
-        <v>9000</v>
+        <v>3500</v>
       </c>
       <c r="H10">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="I10">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="J10">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K10">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L10">
-        <v>500</v>
-      </c>
-      <c r="M10">
-        <v>1000</v>
-      </c>
-      <c r="N10">
-        <v>1500</v>
-      </c>
-      <c r="O10">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="R10" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="11" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A11" s="1">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
+        <v>36</v>
+      </c>
+      <c r="C11" t="s">
+        <v>17</v>
+      </c>
+      <c r="D11" t="s">
+        <v>34</v>
+      </c>
+      <c r="E11" t="s">
         <v>37</v>
-      </c>
-      <c r="B11" t="s">
-        <v>83</v>
-      </c>
-      <c r="C11" t="s">
-        <v>76</v>
-      </c>
-      <c r="D11" t="s">
-        <v>77</v>
-      </c>
-      <c r="E11" t="s">
-        <v>84</v>
       </c>
       <c r="F11" t="s">
         <v>20</v>
@@ -1219,107 +1207,86 @@
         <v>9000</v>
       </c>
       <c r="H11">
-        <v>8</v>
+        <v>3</v>
       </c>
       <c r="I11">
-        <v>2000</v>
+        <v>3000</v>
       </c>
       <c r="J11">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="K11">
-        <v>1000</v>
-      </c>
-      <c r="L11">
-        <v>500</v>
-      </c>
-      <c r="M11">
-        <v>500</v>
-      </c>
-      <c r="N11">
-        <v>1000</v>
-      </c>
-      <c r="O11">
-        <v>1000</v>
-      </c>
-      <c r="P11">
-        <v>1500</v>
+        <v>3000</v>
       </c>
       <c r="R11" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="12" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A12" s="1">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
         <v>40</v>
       </c>
-      <c r="B12" t="s">
-        <v>89</v>
-      </c>
       <c r="C12" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D12" t="s">
-        <v>77</v>
+        <v>34</v>
       </c>
       <c r="E12" t="s">
-        <v>90</v>
+        <v>19</v>
       </c>
       <c r="F12" t="s">
         <v>20</v>
       </c>
       <c r="G12">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H12">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I12">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J12">
+        <v>1000</v>
+      </c>
+      <c r="K12">
+        <v>1000</v>
+      </c>
+      <c r="L12">
         <v>1500</v>
       </c>
-      <c r="K12">
-        <v>1000</v>
-      </c>
-      <c r="L12">
-        <v>1000</v>
-      </c>
-      <c r="M12">
-        <v>1500</v>
-      </c>
-      <c r="N12">
-        <v>2000</v>
-      </c>
       <c r="R12" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="13" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A13" s="1">
-        <v>44</v>
+        <v>12</v>
       </c>
       <c r="B13" t="s">
-        <v>99</v>
+        <v>41</v>
       </c>
       <c r="C13" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D13" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="E13" t="s">
-        <v>100</v>
+        <v>19</v>
       </c>
       <c r="F13" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G13">
-        <v>9000</v>
+        <v>4000</v>
       </c>
       <c r="H13">
-        <v>6</v>
+        <v>3</v>
       </c>
       <c r="I13">
         <v>2000</v>
@@ -1330,57 +1297,57 @@
       <c r="K13">
         <v>1000</v>
       </c>
-      <c r="L13">
-        <v>2000</v>
-      </c>
-      <c r="M13">
-        <v>1500</v>
-      </c>
-      <c r="N13">
-        <v>1500</v>
-      </c>
       <c r="R13" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="14" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A14" s="1">
-        <v>45</v>
+        <v>13</v>
       </c>
       <c r="B14" t="s">
-        <v>101</v>
+        <v>42</v>
       </c>
       <c r="C14" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D14" t="s">
-        <v>93</v>
+        <v>34</v>
       </c>
       <c r="E14" t="s">
-        <v>102</v>
+        <v>43</v>
       </c>
       <c r="F14" t="s">
         <v>20</v>
       </c>
       <c r="G14">
-        <v>9000</v>
+        <v>3500</v>
       </c>
       <c r="H14">
-        <v>1</v>
+        <v>4</v>
       </c>
       <c r="I14">
-        <v>9000</v>
+        <v>2000</v>
+      </c>
+      <c r="J14">
+        <v>500</v>
+      </c>
+      <c r="K14">
+        <v>500</v>
+      </c>
+      <c r="L14">
+        <v>500</v>
       </c>
       <c r="R14" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="15" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A15" s="1">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B15" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="C15" t="s">
         <v>17</v>
@@ -1389,40 +1356,31 @@
         <v>45</v>
       </c>
       <c r="E15" t="s">
-        <v>47</v>
+        <v>19</v>
       </c>
       <c r="F15" t="s">
         <v>20</v>
       </c>
       <c r="G15">
-        <v>7600</v>
+        <v>4000</v>
       </c>
       <c r="H15">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I15">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J15">
-        <v>1500</v>
+        <v>1000</v>
       </c>
       <c r="K15">
         <v>1000</v>
       </c>
       <c r="L15">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M15">
         <v>500</v>
-      </c>
-      <c r="N15">
-        <v>1000</v>
-      </c>
-      <c r="O15">
-        <v>1000</v>
-      </c>
-      <c r="P15">
-        <v>100</v>
       </c>
       <c r="R15" t="s">
         <v>104</v>
@@ -1430,25 +1388,25 @@
     </row>
     <row r="16" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A16" s="1">
-        <v>1</v>
+        <v>15</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>46</v>
       </c>
       <c r="C16" t="s">
         <v>17</v>
       </c>
       <c r="D16" t="s">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="E16" t="s">
-        <v>22</v>
+        <v>47</v>
       </c>
       <c r="F16" t="s">
         <v>20</v>
       </c>
       <c r="G16">
-        <v>7500</v>
+        <v>7600</v>
       </c>
       <c r="H16">
         <v>8</v>
@@ -1457,25 +1415,25 @@
         <v>2000</v>
       </c>
       <c r="J16">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K16">
         <v>1000</v>
       </c>
       <c r="L16">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M16">
         <v>500</v>
       </c>
       <c r="N16">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="O16">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="P16">
-        <v>1000</v>
+        <v>100</v>
       </c>
       <c r="R16" t="s">
         <v>104</v>
@@ -1536,28 +1494,28 @@
     </row>
     <row r="18" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A18" s="1">
-        <v>39</v>
+        <v>17</v>
       </c>
       <c r="B18" t="s">
-        <v>87</v>
+        <v>50</v>
       </c>
       <c r="C18" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D18" t="s">
-        <v>77</v>
+        <v>51</v>
       </c>
       <c r="E18" t="s">
-        <v>88</v>
+        <v>52</v>
       </c>
       <c r="F18" t="s">
         <v>20</v>
       </c>
       <c r="G18">
-        <v>7500</v>
+        <v>9000</v>
       </c>
       <c r="H18">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="I18">
         <v>2000</v>
@@ -1566,51 +1524,48 @@
         <v>1500</v>
       </c>
       <c r="K18">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L18">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M18">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="N18">
-        <v>1000</v>
-      </c>
-      <c r="O18">
-        <v>1500</v>
+        <v>2000</v>
       </c>
       <c r="R18" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="19" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A19" s="1">
-        <v>41</v>
+        <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>91</v>
+        <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D19" t="s">
-        <v>93</v>
+        <v>51</v>
       </c>
       <c r="E19" t="s">
-        <v>94</v>
+        <v>19</v>
       </c>
       <c r="F19" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G19">
-        <v>7500</v>
+        <v>4000</v>
       </c>
       <c r="H19">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="I19">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J19">
         <v>500</v>
@@ -1622,33 +1577,24 @@
         <v>500</v>
       </c>
       <c r="M19">
-        <v>1000</v>
-      </c>
-      <c r="N19">
-        <v>500</v>
-      </c>
-      <c r="O19">
-        <v>1000</v>
-      </c>
-      <c r="P19">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R19" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="20" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A20" s="1">
-        <v>7</v>
+        <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>33</v>
+        <v>55</v>
       </c>
       <c r="C20" t="s">
         <v>17</v>
       </c>
       <c r="D20" t="s">
-        <v>34</v>
+        <v>51</v>
       </c>
       <c r="E20" t="s">
         <v>19</v>
@@ -1657,22 +1603,25 @@
         <v>20</v>
       </c>
       <c r="G20">
-        <v>6500</v>
+        <v>4000</v>
       </c>
       <c r="H20">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I20">
-        <v>2500</v>
+        <v>500</v>
       </c>
       <c r="J20">
-        <v>1500</v>
+        <v>500</v>
       </c>
       <c r="K20">
         <v>1000</v>
       </c>
       <c r="L20">
-        <v>1500</v>
+        <v>1000</v>
+      </c>
+      <c r="M20">
+        <v>1000</v>
       </c>
       <c r="R20" t="s">
         <v>104</v>
@@ -1680,49 +1629,52 @@
     </row>
     <row r="21" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A21" s="1">
-        <v>6</v>
+        <v>24</v>
       </c>
       <c r="B21" t="s">
-        <v>30</v>
+        <v>61</v>
       </c>
       <c r="C21" t="s">
         <v>17</v>
       </c>
       <c r="D21" t="s">
-        <v>31</v>
+        <v>59</v>
       </c>
       <c r="E21" t="s">
-        <v>32</v>
+        <v>62</v>
       </c>
       <c r="F21" t="s">
         <v>20</v>
       </c>
       <c r="G21">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="H21">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="I21">
+        <v>2000</v>
+      </c>
+      <c r="J21">
+        <v>1000</v>
+      </c>
+      <c r="K21">
+        <v>500</v>
+      </c>
+      <c r="L21">
+        <v>1000</v>
+      </c>
+      <c r="M21">
+        <v>1000</v>
+      </c>
+      <c r="N21">
         <v>1500</v>
       </c>
-      <c r="J21">
-        <v>1000</v>
-      </c>
-      <c r="K21">
-        <v>500</v>
-      </c>
-      <c r="L21">
-        <v>500</v>
-      </c>
-      <c r="M21">
-        <v>500</v>
-      </c>
-      <c r="N21">
-        <v>1000</v>
-      </c>
       <c r="O21">
-        <v>1000</v>
+        <v>500</v>
+      </c>
+      <c r="P21">
+        <v>1500</v>
       </c>
       <c r="R21" t="s">
         <v>104</v>
@@ -1730,82 +1682,85 @@
     </row>
     <row r="22" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A22" s="1">
-        <v>42</v>
+        <v>26</v>
       </c>
       <c r="B22" t="s">
-        <v>95</v>
+        <v>64</v>
       </c>
       <c r="C22" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D22" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E22" t="s">
-        <v>96</v>
+        <v>66</v>
       </c>
       <c r="F22" t="s">
         <v>20</v>
       </c>
       <c r="G22">
-        <v>6000</v>
+        <v>10000</v>
       </c>
       <c r="H22">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="I22">
+        <v>1000</v>
+      </c>
+      <c r="J22">
+        <v>2500</v>
+      </c>
+      <c r="K22">
         <v>1500</v>
       </c>
-      <c r="J22">
+      <c r="L22">
+        <v>1000</v>
+      </c>
+      <c r="M22">
+        <v>1000</v>
+      </c>
+      <c r="N22">
         <v>1500</v>
       </c>
-      <c r="K22">
-        <v>1000</v>
-      </c>
-      <c r="L22">
-        <v>1000</v>
-      </c>
-      <c r="M22">
-        <v>500</v>
-      </c>
-      <c r="N22">
-        <v>500</v>
+      <c r="O22">
+        <v>1500</v>
       </c>
       <c r="R22" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="23" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A23" s="1">
-        <v>43</v>
+        <v>28</v>
       </c>
       <c r="B23" t="s">
-        <v>97</v>
+        <v>68</v>
       </c>
       <c r="C23" t="s">
-        <v>92</v>
+        <v>17</v>
       </c>
       <c r="D23" t="s">
-        <v>93</v>
+        <v>65</v>
       </c>
       <c r="E23" t="s">
-        <v>98</v>
+        <v>69</v>
       </c>
       <c r="F23" t="s">
         <v>20</v>
       </c>
       <c r="G23">
-        <v>6000</v>
+        <v>9000</v>
       </c>
       <c r="H23">
         <v>7</v>
       </c>
       <c r="I23">
+        <v>2500</v>
+      </c>
+      <c r="J23">
         <v>1500</v>
       </c>
-      <c r="J23">
-        <v>1000</v>
-      </c>
       <c r="K23">
         <v>500</v>
       </c>
@@ -1813,45 +1768,45 @@
         <v>500</v>
       </c>
       <c r="M23">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N23">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="O23">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R23" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
     </row>
     <row r="24" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A24" s="1">
-        <v>4</v>
+        <v>29</v>
       </c>
       <c r="B24" t="s">
-        <v>27</v>
+        <v>70</v>
       </c>
       <c r="C24" t="s">
         <v>17</v>
       </c>
       <c r="D24" t="s">
-        <v>28</v>
+        <v>71</v>
       </c>
       <c r="E24" t="s">
-        <v>19</v>
+        <v>72</v>
       </c>
       <c r="F24" t="s">
         <v>20</v>
       </c>
       <c r="G24">
-        <v>4500</v>
+        <v>10000</v>
       </c>
       <c r="H24">
-        <v>6</v>
+        <v>9</v>
       </c>
       <c r="I24">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J24">
         <v>1000</v>
@@ -1860,13 +1815,22 @@
         <v>1000</v>
       </c>
       <c r="L24">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M24">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="N24">
         <v>500</v>
+      </c>
+      <c r="O24">
+        <v>1000</v>
+      </c>
+      <c r="P24">
+        <v>1000</v>
+      </c>
+      <c r="Q24">
+        <v>2000</v>
       </c>
       <c r="R24" t="s">
         <v>104</v>
@@ -1874,16 +1838,16 @@
     </row>
     <row r="25" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A25" s="1">
-        <v>5</v>
+        <v>32</v>
       </c>
       <c r="B25" t="s">
-        <v>29</v>
+        <v>78</v>
       </c>
       <c r="C25" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D25" t="s">
-        <v>28</v>
+        <v>77</v>
       </c>
       <c r="E25" t="s">
         <v>19</v>
@@ -1892,10 +1856,10 @@
         <v>20</v>
       </c>
       <c r="G25">
-        <v>4500</v>
+        <v>4000</v>
       </c>
       <c r="H25">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="I25">
         <v>1000</v>
@@ -1910,13 +1874,7 @@
         <v>500</v>
       </c>
       <c r="M25">
-        <v>500</v>
-      </c>
-      <c r="N25">
-        <v>500</v>
-      </c>
-      <c r="O25">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="R25" t="s">
         <v>104</v>
@@ -1924,16 +1882,16 @@
     </row>
     <row r="26" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A26" s="1">
-        <v>0</v>
+        <v>33</v>
       </c>
       <c r="B26" t="s">
-        <v>16</v>
+        <v>79</v>
       </c>
       <c r="C26" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D26" t="s">
-        <v>18</v>
+        <v>77</v>
       </c>
       <c r="E26" t="s">
         <v>19</v>
@@ -1948,19 +1906,19 @@
         <v>5</v>
       </c>
       <c r="I26">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J26">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K26">
         <v>1000</v>
       </c>
       <c r="L26">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M26">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="R26" t="s">
         <v>104</v>
@@ -1968,16 +1926,16 @@
     </row>
     <row r="27" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A27" s="1">
-        <v>11</v>
+        <v>34</v>
       </c>
       <c r="B27" t="s">
-        <v>40</v>
+        <v>80</v>
       </c>
       <c r="C27" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D27" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E27" t="s">
         <v>19</v>
@@ -1989,7 +1947,7 @@
         <v>4000</v>
       </c>
       <c r="H27">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I27">
         <v>500</v>
@@ -1998,10 +1956,13 @@
         <v>1000</v>
       </c>
       <c r="K27">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L27">
-        <v>1500</v>
+        <v>1000</v>
+      </c>
+      <c r="M27">
+        <v>1000</v>
       </c>
       <c r="R27" t="s">
         <v>104</v>
@@ -2009,37 +1970,43 @@
     </row>
     <row r="28" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A28" s="1">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B28" t="s">
-        <v>41</v>
+        <v>82</v>
       </c>
       <c r="C28" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D28" t="s">
-        <v>34</v>
+        <v>77</v>
       </c>
       <c r="E28" t="s">
         <v>19</v>
       </c>
       <c r="F28" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G28">
         <v>4000</v>
       </c>
       <c r="H28">
-        <v>3</v>
+        <v>5</v>
       </c>
       <c r="I28">
-        <v>2000</v>
+        <v>500</v>
       </c>
       <c r="J28">
         <v>1000</v>
       </c>
       <c r="K28">
         <v>1000</v>
+      </c>
+      <c r="L28">
+        <v>1000</v>
+      </c>
+      <c r="M28">
+        <v>500</v>
       </c>
       <c r="R28" t="s">
         <v>104</v>
@@ -2047,43 +2014,52 @@
     </row>
     <row r="29" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A29" s="1">
-        <v>14</v>
+        <v>37</v>
       </c>
       <c r="B29" t="s">
-        <v>44</v>
+        <v>83</v>
       </c>
       <c r="C29" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D29" t="s">
-        <v>45</v>
+        <v>77</v>
       </c>
       <c r="E29" t="s">
-        <v>19</v>
+        <v>84</v>
       </c>
       <c r="F29" t="s">
         <v>20</v>
       </c>
       <c r="G29">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="H29">
-        <v>5</v>
+        <v>8</v>
       </c>
       <c r="I29">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J29">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K29">
         <v>1000</v>
       </c>
       <c r="L29">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M29">
         <v>500</v>
+      </c>
+      <c r="N29">
+        <v>1000</v>
+      </c>
+      <c r="O29">
+        <v>1000</v>
+      </c>
+      <c r="P29">
+        <v>1500</v>
       </c>
       <c r="R29" t="s">
         <v>104</v>
@@ -2091,43 +2067,43 @@
     </row>
     <row r="30" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A30" s="1">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="B30" t="s">
-        <v>54</v>
+        <v>85</v>
       </c>
       <c r="C30" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D30" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E30" t="s">
-        <v>19</v>
+        <v>86</v>
       </c>
       <c r="F30" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G30">
-        <v>4000</v>
+        <v>10400</v>
       </c>
       <c r="H30">
         <v>5</v>
       </c>
       <c r="I30">
-        <v>500</v>
+        <v>3000</v>
       </c>
       <c r="J30">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="K30">
-        <v>1000</v>
+        <v>3000</v>
       </c>
       <c r="L30">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M30">
-        <v>1500</v>
+        <v>1400</v>
       </c>
       <c r="R30" t="s">
         <v>104</v>
@@ -2135,34 +2111,34 @@
     </row>
     <row r="31" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A31" s="1">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="B31" t="s">
-        <v>55</v>
+        <v>89</v>
       </c>
       <c r="C31" t="s">
-        <v>17</v>
+        <v>76</v>
       </c>
       <c r="D31" t="s">
-        <v>51</v>
+        <v>77</v>
       </c>
       <c r="E31" t="s">
-        <v>19</v>
+        <v>90</v>
       </c>
       <c r="F31" t="s">
         <v>20</v>
       </c>
       <c r="G31">
-        <v>4000</v>
+        <v>9000</v>
       </c>
       <c r="H31">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I31">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J31">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K31">
         <v>1000</v>
@@ -2171,7 +2147,10 @@
         <v>1000</v>
       </c>
       <c r="M31">
-        <v>1000</v>
+        <v>1500</v>
+      </c>
+      <c r="N31">
+        <v>2000</v>
       </c>
       <c r="R31" t="s">
         <v>104</v>
@@ -2179,45 +2158,39 @@
     </row>
     <row r="32" spans="1:18" x14ac:dyDescent="0.3">
       <c r="A32" s="1">
-        <v>21</v>
+        <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>56</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
         <v>17</v>
       </c>
       <c r="D32" t="s">
-        <v>57</v>
+        <v>34</v>
       </c>
       <c r="E32" t="s">
         <v>19</v>
       </c>
       <c r="F32" t="s">
-        <v>20</v>
+        <v>39</v>
       </c>
       <c r="G32">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="H32">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="I32">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J32">
         <v>500</v>
       </c>
       <c r="K32">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L32">
-        <v>1000</v>
-      </c>
-      <c r="M32">
-        <v>1000</v>
-      </c>
-      <c r="N32">
         <v>500</v>
       </c>
       <c r="R32" t="s">
@@ -2226,16 +2199,16 @@
     </row>
     <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" s="1">
-        <v>22</v>
+        <v>18</v>
       </c>
       <c r="B33" t="s">
-        <v>58</v>
+        <v>53</v>
       </c>
       <c r="C33" t="s">
         <v>17</v>
       </c>
       <c r="D33" t="s">
-        <v>59</v>
+        <v>51</v>
       </c>
       <c r="E33" t="s">
         <v>19</v>
@@ -2244,10 +2217,10 @@
         <v>20</v>
       </c>
       <c r="G33">
-        <v>4000</v>
+        <v>2500</v>
       </c>
       <c r="H33">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I33">
         <v>500</v>
@@ -2256,12 +2229,9 @@
         <v>1000</v>
       </c>
       <c r="K33">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L33">
-        <v>1000</v>
-      </c>
-      <c r="M33">
         <v>500</v>
       </c>
       <c r="R33" t="s">
@@ -2270,16 +2240,16 @@
     </row>
     <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" s="1">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B34" t="s">
-        <v>60</v>
+        <v>56</v>
       </c>
       <c r="C34" t="s">
         <v>17</v>
       </c>
       <c r="D34" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="E34" t="s">
         <v>19</v>
@@ -2303,13 +2273,13 @@
         <v>500</v>
       </c>
       <c r="L34">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M34">
         <v>1000</v>
       </c>
       <c r="N34">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R34" t="s">
         <v>106</v>
@@ -2317,10 +2287,10 @@
     </row>
     <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" s="1">
-        <v>25</v>
+        <v>22</v>
       </c>
       <c r="B35" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
       <c r="C35" t="s">
         <v>17</v>
@@ -2341,19 +2311,19 @@
         <v>5</v>
       </c>
       <c r="I35">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J35">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K35">
         <v>1000</v>
       </c>
       <c r="L35">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M35">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R35" t="s">
         <v>106</v>
@@ -2361,16 +2331,16 @@
     </row>
     <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" s="1">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B36" t="s">
-        <v>67</v>
+        <v>60</v>
       </c>
       <c r="C36" t="s">
         <v>17</v>
       </c>
       <c r="D36" t="s">
-        <v>65</v>
+        <v>59</v>
       </c>
       <c r="E36" t="s">
         <v>19</v>
@@ -2382,22 +2352,25 @@
         <v>4000</v>
       </c>
       <c r="H36">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I36">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J36">
         <v>500</v>
       </c>
       <c r="K36">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L36">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M36">
-        <v>500</v>
+        <v>1000</v>
+      </c>
+      <c r="N36">
+        <v>1000</v>
       </c>
       <c r="R36" t="s">
         <v>106</v>
@@ -2406,16 +2379,16 @@
     </row>
     <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" s="1">
-        <v>30</v>
+        <v>25</v>
       </c>
       <c r="B37" t="s">
-        <v>73</v>
+        <v>63</v>
       </c>
       <c r="C37" t="s">
         <v>17</v>
       </c>
       <c r="D37" t="s">
-        <v>74</v>
+        <v>59</v>
       </c>
       <c r="E37" t="s">
         <v>19</v>
@@ -2427,19 +2400,22 @@
         <v>4000</v>
       </c>
       <c r="H37">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="I37">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J37">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K37">
         <v>1000</v>
       </c>
       <c r="L37">
-        <v>1500</v>
+        <v>500</v>
+      </c>
+      <c r="M37">
+        <v>1000</v>
       </c>
       <c r="R37" t="s">
         <v>106</v>
@@ -2447,16 +2423,16 @@
     </row>
     <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" s="1">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B38" t="s">
-        <v>75</v>
+        <v>67</v>
       </c>
       <c r="C38" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D38" t="s">
-        <v>77</v>
+        <v>65</v>
       </c>
       <c r="E38" t="s">
         <v>19</v>
@@ -2480,10 +2456,10 @@
         <v>1000</v>
       </c>
       <c r="L38">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="M38">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="R38" t="s">
         <v>106</v>
@@ -2494,16 +2470,16 @@
     </row>
     <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" s="1">
-        <v>32</v>
+        <v>30</v>
       </c>
       <c r="B39" t="s">
-        <v>78</v>
+        <v>73</v>
       </c>
       <c r="C39" t="s">
-        <v>76</v>
+        <v>17</v>
       </c>
       <c r="D39" t="s">
-        <v>77</v>
+        <v>74</v>
       </c>
       <c r="E39" t="s">
         <v>19</v>
@@ -2515,33 +2491,30 @@
         <v>4000</v>
       </c>
       <c r="H39">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I39">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="J39">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K39">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L39">
-        <v>500</v>
-      </c>
-      <c r="M39">
         <v>1500</v>
       </c>
       <c r="R39" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" s="1">
-        <v>33</v>
+        <v>31</v>
       </c>
       <c r="B40" t="s">
-        <v>79</v>
+        <v>75</v>
       </c>
       <c r="C40" t="s">
         <v>76</v>
@@ -2577,15 +2550,15 @@
         <v>1000</v>
       </c>
       <c r="R40" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" s="1">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B41" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="C41" t="s">
         <v>76</v>
@@ -2600,16 +2573,16 @@
         <v>20</v>
       </c>
       <c r="G41">
-        <v>4000</v>
+        <v>3000</v>
       </c>
       <c r="H41">
-        <v>5</v>
+        <v>4</v>
       </c>
       <c r="I41">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="J41">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K41">
         <v>500</v>
@@ -2617,19 +2590,16 @@
       <c r="L41">
         <v>1000</v>
       </c>
-      <c r="M41">
-        <v>1000</v>
-      </c>
       <c r="R41" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" s="1">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B42" t="s">
-        <v>82</v>
+        <v>87</v>
       </c>
       <c r="C42" t="s">
         <v>76</v>
@@ -2638,154 +2608,187 @@
         <v>77</v>
       </c>
       <c r="E42" t="s">
-        <v>19</v>
+        <v>88</v>
       </c>
       <c r="F42" t="s">
         <v>20</v>
       </c>
       <c r="G42">
-        <v>4000</v>
+        <v>7500</v>
       </c>
       <c r="H42">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="I42">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J42">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="K42">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L42">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="M42">
         <v>500</v>
       </c>
+      <c r="N42">
+        <v>1000</v>
+      </c>
+      <c r="O42">
+        <v>1500</v>
+      </c>
       <c r="R42" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" s="1">
+        <v>41</v>
+      </c>
+      <c r="B43" t="s">
+        <v>91</v>
+      </c>
+      <c r="C43" t="s">
+        <v>92</v>
+      </c>
+      <c r="D43" t="s">
+        <v>93</v>
+      </c>
+      <c r="E43" t="s">
+        <v>94</v>
+      </c>
+      <c r="F43" t="s">
+        <v>20</v>
+      </c>
+      <c r="G43">
+        <v>7500</v>
+      </c>
+      <c r="H43">
         <v>8</v>
       </c>
-      <c r="B43" t="s">
-        <v>35</v>
-      </c>
-      <c r="C43" t="s">
-        <v>17</v>
-      </c>
-      <c r="D43" t="s">
-        <v>34</v>
-      </c>
-      <c r="E43" t="s">
-        <v>19</v>
-      </c>
-      <c r="F43" t="s">
-        <v>20</v>
-      </c>
-      <c r="G43">
-        <v>3500</v>
-      </c>
-      <c r="H43">
-        <v>4</v>
-      </c>
       <c r="I43">
-        <v>500</v>
+        <v>2000</v>
       </c>
       <c r="J43">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="K43">
         <v>1000</v>
       </c>
       <c r="L43">
+        <v>500</v>
+      </c>
+      <c r="M43">
+        <v>1000</v>
+      </c>
+      <c r="N43">
+        <v>500</v>
+      </c>
+      <c r="O43">
+        <v>1000</v>
+      </c>
+      <c r="P43">
         <v>1000</v>
       </c>
       <c r="R43" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" s="1">
-        <v>13</v>
+        <v>42</v>
       </c>
       <c r="B44" t="s">
-        <v>42</v>
+        <v>95</v>
       </c>
       <c r="C44" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D44" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E44" t="s">
-        <v>43</v>
+        <v>96</v>
       </c>
       <c r="F44" t="s">
         <v>20</v>
       </c>
       <c r="G44">
-        <v>3500</v>
+        <v>6000</v>
       </c>
       <c r="H44">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I44">
-        <v>2000</v>
+        <v>1500</v>
       </c>
       <c r="J44">
-        <v>500</v>
+        <v>1500</v>
       </c>
       <c r="K44">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L44">
+        <v>1000</v>
+      </c>
+      <c r="M44">
+        <v>500</v>
+      </c>
+      <c r="N44">
         <v>500</v>
       </c>
       <c r="R44" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
     </row>
     <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" s="1">
-        <v>10</v>
+        <v>43</v>
       </c>
       <c r="B45" t="s">
-        <v>38</v>
+        <v>97</v>
       </c>
       <c r="C45" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D45" t="s">
-        <v>34</v>
+        <v>93</v>
       </c>
       <c r="E45" t="s">
-        <v>19</v>
+        <v>98</v>
       </c>
       <c r="F45" t="s">
-        <v>39</v>
+        <v>20</v>
       </c>
       <c r="G45">
-        <v>3000</v>
+        <v>6000</v>
       </c>
       <c r="H45">
-        <v>4</v>
+        <v>7</v>
       </c>
       <c r="I45">
-        <v>1000</v>
+        <v>1500</v>
       </c>
       <c r="J45">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K45">
-        <v>1000</v>
+        <v>500</v>
       </c>
       <c r="L45">
         <v>500</v>
+      </c>
+      <c r="M45">
+        <v>500</v>
+      </c>
+      <c r="N45">
+        <v>1000</v>
+      </c>
+      <c r="O45">
+        <v>1000</v>
       </c>
       <c r="R45" t="s">
         <v>106</v>
@@ -2793,40 +2796,46 @@
     </row>
     <row r="46" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A46" s="1">
-        <v>35</v>
+        <v>44</v>
       </c>
       <c r="B46" t="s">
-        <v>81</v>
+        <v>99</v>
       </c>
       <c r="C46" t="s">
-        <v>76</v>
+        <v>92</v>
       </c>
       <c r="D46" t="s">
-        <v>77</v>
+        <v>93</v>
       </c>
       <c r="E46" t="s">
-        <v>19</v>
+        <v>100</v>
       </c>
       <c r="F46" t="s">
         <v>20</v>
       </c>
       <c r="G46">
-        <v>3000</v>
+        <v>9000</v>
       </c>
       <c r="H46">
-        <v>4</v>
+        <v>6</v>
       </c>
       <c r="I46">
-        <v>1000</v>
+        <v>2000</v>
       </c>
       <c r="J46">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="K46">
-        <v>500</v>
+        <v>1000</v>
       </c>
       <c r="L46">
-        <v>1000</v>
+        <v>2000</v>
+      </c>
+      <c r="M46">
+        <v>1500</v>
+      </c>
+      <c r="N46">
+        <v>1500</v>
       </c>
       <c r="R46" t="s">
         <v>106</v>
@@ -2834,53 +2843,39 @@
     </row>
     <row r="47" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A47" s="1">
-        <v>18</v>
+        <v>45</v>
       </c>
       <c r="B47" t="s">
-        <v>53</v>
+        <v>101</v>
       </c>
       <c r="C47" t="s">
-        <v>17</v>
+        <v>92</v>
       </c>
       <c r="D47" t="s">
-        <v>51</v>
+        <v>93</v>
       </c>
       <c r="E47" t="s">
-        <v>19</v>
+        <v>102</v>
       </c>
       <c r="F47" t="s">
         <v>20</v>
       </c>
       <c r="G47">
-        <v>2500</v>
+        <v>9000</v>
       </c>
       <c r="H47">
-        <v>4</v>
+        <v>1</v>
       </c>
       <c r="I47">
-        <v>500</v>
-      </c>
-      <c r="J47">
-        <v>1000</v>
-      </c>
-      <c r="K47">
-        <v>500</v>
-      </c>
-      <c r="L47">
-        <v>500</v>
+        <v>9000</v>
       </c>
       <c r="R47" t="s">
         <v>106</v>
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:R47" xr:uid="{00000000-0001-0000-0000-000000000000}">
-    <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R47">
-      <sortCondition descending="1" ref="G1:G47"/>
-    </sortState>
-  </autoFilter>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:R47">
-    <sortCondition ref="A1:A47"/>
+    <sortCondition descending="1" ref="R1:R47"/>
   </sortState>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>

</xml_diff>